<commit_message>
Fix missing slots and add attributes
</commit_message>
<xml_diff>
--- a/minimal_1/metadata.xlsx
+++ b/minimal_1/metadata.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/dev/example-data/minimal_1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/tmp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9FAD8D00-21AA-8644-A4DD-46C9D3ECFC8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80D1B05A-2EAF-3940-8ECD-7CB5D7AC33D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20640" yWindow="500" windowWidth="30560" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7740" yWindow="5300" windowWidth="23800" windowHeight="23520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Study" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="646" uniqueCount="275">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="649" uniqueCount="278">
   <si>
     <t>alias</t>
   </si>
@@ -852,6 +852,15 @@
   <si>
     <t>The DAC institute</t>
   </si>
+  <si>
+    <t>A Type</t>
+  </si>
+  <si>
+    <t>Some Institute</t>
+  </si>
+  <si>
+    <t>budget=3.5M;funding=EU</t>
+  </si>
 </sst>
 </file>
 
@@ -1329,8 +1338,8 @@
   </sheetPr>
   <dimension ref="A1:F1006"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1474,7 +1483,9 @@
       <c r="E7" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="F7" s="3"/>
+      <c r="F7" s="3" t="s">
+        <v>277</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
@@ -1489,7 +1500,9 @@
       <c r="D8" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="E8" s="3"/>
+      <c r="E8" s="3" t="s">
+        <v>276</v>
+      </c>
       <c r="F8" s="3"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -20498,7 +20511,7 @@
   <dimension ref="A1:E1006"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:E10"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -20669,7 +20682,9 @@
       <c r="C10" s="9" t="s">
         <v>258</v>
       </c>
-      <c r="D10" s="9"/>
+      <c r="D10" s="9" t="s">
+        <v>275</v>
+      </c>
       <c r="E10" s="9" t="s">
         <v>259</v>
       </c>

</xml_diff>

<commit_message>
Fix missing slots and add attributes (#5)
</commit_message>
<xml_diff>
--- a/minimal_1/metadata.xlsx
+++ b/minimal_1/metadata.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/dev/example-data/minimal_1/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/tmp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9FAD8D00-21AA-8644-A4DD-46C9D3ECFC8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80D1B05A-2EAF-3940-8ECD-7CB5D7AC33D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20640" yWindow="500" windowWidth="30560" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7740" yWindow="5300" windowWidth="23800" windowHeight="23520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Study" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="646" uniqueCount="275">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="649" uniqueCount="278">
   <si>
     <t>alias</t>
   </si>
@@ -852,6 +852,15 @@
   <si>
     <t>The DAC institute</t>
   </si>
+  <si>
+    <t>A Type</t>
+  </si>
+  <si>
+    <t>Some Institute</t>
+  </si>
+  <si>
+    <t>budget=3.5M;funding=EU</t>
+  </si>
 </sst>
 </file>
 
@@ -1329,8 +1338,8 @@
   </sheetPr>
   <dimension ref="A1:F1006"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1474,7 +1483,9 @@
       <c r="E7" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="F7" s="3"/>
+      <c r="F7" s="3" t="s">
+        <v>277</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
@@ -1489,7 +1500,9 @@
       <c r="D8" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="E8" s="3"/>
+      <c r="E8" s="3" t="s">
+        <v>276</v>
+      </c>
       <c r="F8" s="3"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -20498,7 +20511,7 @@
   <dimension ref="A1:E1006"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:E10"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -20669,7 +20682,9 @@
       <c r="C10" s="9" t="s">
         <v>258</v>
       </c>
-      <c r="D10" s="9"/>
+      <c r="D10" s="9" t="s">
+        <v>275</v>
+      </c>
       <c r="E10" s="9" t="s">
         <v>259</v>
       </c>

</xml_diff>

<commit_message>
Slightly enlarge minimal_1 filesizes and move filename content to beginning
</commit_message>
<xml_diff>
--- a/minimal_1/metadata.xlsx
+++ b/minimal_1/metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/dev/example-data/minimal_1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{940C727C-6C82-6040-8232-F5EA0245E7F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFA2D7B8-8CE6-1146-9BEF-A124E6ECA0F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="27300" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -317,9 +317,6 @@
     <t>FASTQ</t>
   </si>
   <si>
-    <t>07611c4987b9e5be1304a992dbc25242824acf808c829819732a8f5f6c40e731</t>
-  </si>
-  <si>
     <t>SHA256</t>
   </si>
   <si>
@@ -332,16 +329,10 @@
     <t>SEQ_FILE_A_R2.fastq.gz</t>
   </si>
   <si>
-    <t>ba7f0fa2da3c1bd473b01985c2fd25175d55f1edb27e530d735ff85ed187c122</t>
-  </si>
-  <si>
     <t>FILE_3</t>
   </si>
   <si>
     <t>SEQ_FILE_B_R1.fastq.gz</t>
-  </si>
-  <si>
-    <t>cbfa35d3a7d83b4ae5e3b06b04f3d784f2094497d434c9e6b50ac36753ee0025</t>
   </si>
   <si>
     <t>FILE_4</t>
@@ -350,16 +341,10 @@
     <t>SEQ_FILE_B_R2.fastq.gz</t>
   </si>
   <si>
-    <t>d42f211b7c589961332f86a2a41945ef9f3dd8ffc01a34d7755c27f7eb5b0bdb</t>
-  </si>
-  <si>
     <t>FILE_5</t>
   </si>
   <si>
     <t>SEQ_FILE_C_R1.fastq.gz</t>
-  </si>
-  <si>
-    <t>299585554663327257bd92a624760a3cbb009804a910ba03fc977d297d62ec7f</t>
   </si>
   <si>
     <t>FILE_6</t>
@@ -368,16 +353,10 @@
     <t>SEQ_FILE_C_R2.fastq.gz</t>
   </si>
   <si>
-    <t>83b23fb63eaa7dd8fed5447cc719077412bcb7cd5a82e710bae56643c00f27a2</t>
-  </si>
-  <si>
     <t>FILE_7</t>
   </si>
   <si>
     <t>SEQ_FILE_D_R1.fastq.gz</t>
-  </si>
-  <si>
-    <t>35f68cc8abc534f8ccb7e827aa4ab0f5d3736c310701144217e433af86c2f132</t>
   </si>
   <si>
     <t>FILE_8</t>
@@ -386,16 +365,10 @@
     <t>SEQ_FILE_D_R2.fastq.gz</t>
   </si>
   <si>
-    <t>05d1ed4457580cafab18e3cc06c8cac3bd1c6def191704e70c7e11d221b69f12</t>
-  </si>
-  <si>
     <t>FILE_9</t>
   </si>
   <si>
     <t>SEQ_FILE_E_R1.fastq.gz</t>
-  </si>
-  <si>
-    <t>cd230d8cf3bcdd10292a54cccc5c168dfec1d51b416ddc5102cbea259f3562bd</t>
   </si>
   <si>
     <t>FILE_10</t>
@@ -404,16 +377,10 @@
     <t>SEQ_FILE_E_R2.fastq.gz</t>
   </si>
   <si>
-    <t>7bdf0cb577c4b08a0890ece353a287493ea46c1fd8a2f9e27cb267be8c89c06c</t>
-  </si>
-  <si>
     <t>FILE_11</t>
   </si>
   <si>
     <t>SEQ_FILE_F_R1.fastq.gz</t>
-  </si>
-  <si>
-    <t>e383dd77d2e758d6373bff3abf501011fe6fb5c7af3089fd27abf367d4a92df9</t>
   </si>
   <si>
     <t>FILE_12</t>
@@ -422,16 +389,10 @@
     <t>SEQ_FILE_F_R2.fastq.gz</t>
   </si>
   <si>
-    <t>7729bc30f812e9ec967f89b3a1ad96f9290ffb92148baed608f520137a9fcff2</t>
-  </si>
-  <si>
     <t>FILE_13</t>
   </si>
   <si>
     <t>SEQ_FILE_G_R1.fastq.gz</t>
-  </si>
-  <si>
-    <t>e4bdbee6ace3161310e2b2f1eb16486509c6152f75f8c4da6d255289cd463943</t>
   </si>
   <si>
     <t>FILE_14</t>
@@ -440,16 +401,10 @@
     <t>SEQ_FILE_G_R2.fastq.gz</t>
   </si>
   <si>
-    <t>1dd5ca9bff0f1a48ee4c423a07cb7fd4e53c4c253d9e6d389e35d3be3e215e4e</t>
-  </si>
-  <si>
     <t>FILE_15</t>
   </si>
   <si>
     <t>SEQ_FILE_H_R1.fastq.gz</t>
-  </si>
-  <si>
-    <t>8d214cc1d2556bc6111de52e785ca1cde68b0fb024da219841552e328351ff3b</t>
   </si>
   <si>
     <t>FILE_16</t>
@@ -458,16 +413,10 @@
     <t>SEQ_FILE_H_R2.fastq.gz</t>
   </si>
   <si>
-    <t>358599ff0a1f1f15ce42b484496bc8dafb66ac07f2ab55ba0e2482e191ca5747</t>
-  </si>
-  <si>
     <t>FILE_17</t>
   </si>
   <si>
     <t>SEQ_FILE_I_R1.fastq.gz</t>
-  </si>
-  <si>
-    <t>b7fd9aca6c35f44baab8a8f750049620c5ccff3b4ce300ff9a282682a7302a65</t>
   </si>
   <si>
     <t>DS_2</t>
@@ -479,16 +428,10 @@
     <t>SEQ_FILE_I_R2.fastq.gz</t>
   </si>
   <si>
-    <t>2f660b9617185b44d2ec186eaf6299a43e8860a986077f9961e6ed87fea64824</t>
-  </si>
-  <si>
     <t>FILE_19</t>
   </si>
   <si>
     <t>SEQ_FILE_J_R1.fastq.gz</t>
-  </si>
-  <si>
-    <t>fec3b1b125f5270ff644c7e197494e8f0f20d8d5666065891cdfa3a9b6afd088</t>
   </si>
   <si>
     <t>FILE_20</t>
@@ -497,16 +440,10 @@
     <t>SEQ_FILE_J_R2.fastq.gz</t>
   </si>
   <si>
-    <t>03aa21f81b69d9484d58d9fcd7b6f10f3c2921d02034053fd89746742d0b48db</t>
-  </si>
-  <si>
     <t>FILE_21</t>
   </si>
   <si>
     <t>SEQ_FILE_K_R1.fastq.gz</t>
-  </si>
-  <si>
-    <t>96a4fe6942d341f74d18bd1c9d02e4af3327e18242591434024101dceafc6d4c</t>
   </si>
   <si>
     <t>FILE_22</t>
@@ -515,16 +452,10 @@
     <t>SEQ_FILE_K_R2.fastq.gz</t>
   </si>
   <si>
-    <t>4f8b52e0e874bfe1ae8813cbde44a102b85462f4ffb95c08f147771d0d5a5ae5</t>
-  </si>
-  <si>
     <t>FILE_23</t>
   </si>
   <si>
     <t>SEQ_FILE_L_R1.fastq.gz</t>
-  </si>
-  <si>
-    <t>a65dca5defc93dea1164839398df8a01a32370234a35a146a78018c2155c3b04</t>
   </si>
   <si>
     <t>DS_3</t>
@@ -536,16 +467,10 @@
     <t>SEQ_FILE_L_R2.fastq.gz</t>
   </si>
   <si>
-    <t>f42fa32c6bae7d38e4fe613fcca2f82952ffcb88d422bc2271bcb07bdbc51d9c</t>
-  </si>
-  <si>
     <t>FILE_25</t>
   </si>
   <si>
     <t>SEQ_FILE_M_R1.fastq.gz</t>
-  </si>
-  <si>
-    <t>6aa0b2825179a9998f78b11dcefefde944e21d7f45ee71a4e998ee9b94fc6ed4</t>
   </si>
   <si>
     <t>FILE_26</t>
@@ -554,16 +479,10 @@
     <t>SEQ_FILE_M_R2.fastq.gz</t>
   </si>
   <si>
-    <t>82f8ef5f7bd14703ca7e8a63f7bd10b9910bb195dc7fefdeb86794078a809d5e</t>
-  </si>
-  <si>
     <t>FILE_27</t>
   </si>
   <si>
     <t>SEQ_FILE_N_R1.fastq.gz</t>
-  </si>
-  <si>
-    <t>b25f7ae42b96cd6f0ad2bd797ae3a7e53e7e662786f2ffe1fe6bb1a8dfe7096b</t>
   </si>
   <si>
     <t>FILE_28</t>
@@ -572,16 +491,10 @@
     <t>SEQ_FILE_N_R2.fastq.gz</t>
   </si>
   <si>
-    <t>82be207843fb30084226cea0ae64e8247f84b4592a6b3539aa756dd871b54f96</t>
-  </si>
-  <si>
     <t>FILE_29</t>
   </si>
   <si>
     <t>SEQ_FILE_O_R1.fastq.gz</t>
-  </si>
-  <si>
-    <t>40a64a7c104f67ccf6521af0d25644c0adf270db11e322172a19e5576f9e9db7</t>
   </si>
   <si>
     <t>FILE_30</t>
@@ -590,16 +503,10 @@
     <t>SEQ_FILE_O_R2.fastq.gz</t>
   </si>
   <si>
-    <t>0b0663e0391b1d2b3b513be5981030a5b34337c4cfb4b978bfa07e04f48ecfe9</t>
-  </si>
-  <si>
     <t>FILE_31</t>
   </si>
   <si>
     <t>SEQ_FILE_P_R1.fastq.gz</t>
-  </si>
-  <si>
-    <t>ec8d0dfd3815bd2d2db636432d9d5471522a8b34c8429728e67319672f0e293f</t>
   </si>
   <si>
     <t>FILE_32</t>
@@ -608,16 +515,10 @@
     <t>SEQ_FILE_P_R2.fastq.gz</t>
   </si>
   <si>
-    <t>30439ff89fe2b9a373fcaac3c8bb1bfa912381c675d7663112ee922768170f8e</t>
-  </si>
-  <si>
     <t>FILE_33</t>
   </si>
   <si>
     <t>SEQ_FILE_Q_R1.fastq.gz</t>
-  </si>
-  <si>
-    <t>f54a61941105b510acafd91f9392efd5a3d8cc7f965960983e0cbfe03b2cc11d</t>
   </si>
   <si>
     <t>FILE_34</t>
@@ -626,16 +527,10 @@
     <t>SEQ_FILE_Q_R2.fastq.gz</t>
   </si>
   <si>
-    <t>060c20d2a467b08bf76b7b02db890ab731397d1bb3ddd951b38e72b12574cee5</t>
-  </si>
-  <si>
     <t>FILE_35</t>
   </si>
   <si>
     <t>SEQ_FILE_R_R1.fastq.gz</t>
-  </si>
-  <si>
-    <t>dc9ede6ab543d7d9ef796f074e912f589de847f62b9ec4742464110bf76a8e34</t>
   </si>
   <si>
     <t>FILE_36</t>
@@ -644,16 +539,10 @@
     <t>SEQ_FILE_R_R2.fastq.gz</t>
   </si>
   <si>
-    <t>2c04f666c91335b412dcf9b397d702edd2b26c7eda8b11547c7e76fb37752939</t>
-  </si>
-  <si>
     <t>FILE_37</t>
   </si>
   <si>
     <t>SEQ_FILE_S_R1.fastq.gz</t>
-  </si>
-  <si>
-    <t>e4c1abf47f7bd43bf7d341247392f27439aaa2b17d003a2aceb2b5b83bcd6d45</t>
   </si>
   <si>
     <t>FILE_38</t>
@@ -662,16 +551,10 @@
     <t>SEQ_FILE_S_R2.fastq.gz</t>
   </si>
   <si>
-    <t>83e3dfc7970238c7c3210dd4adaff223a1ccb4cdabbd19c91e217c02a31bd130</t>
-  </si>
-  <si>
     <t>FILE_39</t>
   </si>
   <si>
     <t>SEQ_FILE_T_R1.fastq.gz</t>
-  </si>
-  <si>
-    <t>d2206c38a47a85b8aec9b1be37f8c0e63a0d42689341e4b82ebce4dcd2195293</t>
   </si>
   <si>
     <t>FILE_40</t>
@@ -680,16 +563,10 @@
     <t>SEQ_FILE_T_R2.fastq.gz</t>
   </si>
   <si>
-    <t>07d5f9da9d4b50c419664fad70fb08773b1a81677adcc754bf04f43890d4c4fc</t>
-  </si>
-  <si>
     <t>FILE_41</t>
   </si>
   <si>
     <t>SEQ_FILE_U_R1.fastq.gz</t>
-  </si>
-  <si>
-    <t>65c50feed58a44b9bbe2f14185e0de2e5a9e0868fa25f4be4dd119a2e2b3fdaf</t>
   </si>
   <si>
     <t>FILE_42</t>
@@ -698,16 +575,10 @@
     <t>SEQ_FILE_U_R2.fastq.gz</t>
   </si>
   <si>
-    <t>1d6c077b6f5dbb8032858bdbd530c56b7ac6b1c4feb4be4a155ed456c4d01f1a</t>
-  </si>
-  <si>
     <t>FILE_43</t>
   </si>
   <si>
     <t>SEQ_FILE_V_R1.fastq.gz</t>
-  </si>
-  <si>
-    <t>236b00280ba6301fcc801473e2061ffa33215bc17579108ce99f197742959eb4</t>
   </si>
   <si>
     <t>DS_4</t>
@@ -719,16 +590,10 @@
     <t>SEQ_FILE_V_R2.fastq.gz</t>
   </si>
   <si>
-    <t>14888f079a8464a28370ff4aea9382cf94dd8155f77677b2c49deb8c249ce957</t>
-  </si>
-  <si>
     <t>FILE_45</t>
   </si>
   <si>
     <t>SEQ_FILE_W_R1.fastq.gz</t>
-  </si>
-  <si>
-    <t>cef8667aac74dd8cd057d087ffbddd3d1c8a653b6e595ce9a3cc567e013a0097</t>
   </si>
   <si>
     <t>FILE_46</t>
@@ -737,16 +602,10 @@
     <t>SEQ_FILE_W_R2.fastq.gz</t>
   </si>
   <si>
-    <t>333459bc3f4c12ca8f2f21d81d3883b15843e0e3b8497c213b1808693e927337</t>
-  </si>
-  <si>
     <t>FILE_47</t>
   </si>
   <si>
     <t>SEQ_FILE_X_R1.fastq.gz</t>
-  </si>
-  <si>
-    <t>2df56e140d380e0fedaf11a5a9789418250c2c1397c26b268f214ab9912d720c</t>
   </si>
   <si>
     <t>FILE_48</t>
@@ -755,16 +614,10 @@
     <t>SEQ_FILE_X_R2.fastq.gz</t>
   </si>
   <si>
-    <t>6951e467a10b198a699b7313e11a71cbc35eb968a9e98c2b6014f42b56120e1f</t>
-  </si>
-  <si>
     <t>FILE_49</t>
   </si>
   <si>
     <t>SEQ_FILE_Y_R1.fastq.gz</t>
-  </si>
-  <si>
-    <t>e50386fcd750c0e101a4910db71d2c825d0149e0b41ff701405191c514e493c5</t>
   </si>
   <si>
     <t>FILE_50</t>
@@ -773,25 +626,16 @@
     <t>SEQ_FILE_Y_R2.fastq.gz</t>
   </si>
   <si>
-    <t>80c54f88047174aed9f0354fefc8a8ba4cec2c0422eb03c627e902db7af7c70d</t>
-  </si>
-  <si>
     <t>FILE_51</t>
   </si>
   <si>
     <t>SEQ_FILE_Z_R1.fastq.gz</t>
   </si>
   <si>
-    <t>21bba04d8308dd3a46acd4da5aa67f14e13358fc8a3f84aa12b23a50d426dc7a</t>
-  </si>
-  <si>
     <t>FILE_52</t>
   </si>
   <si>
     <t>SEQ_FILE_Z_R2.fastq.gz</t>
-  </si>
-  <si>
-    <t>63175ec704f31428a49b21464d64746259f809c9669531def763b396e3641da9</t>
   </si>
   <si>
     <t>FORWARD</t>
@@ -885,6 +729,162 @@
   </si>
   <si>
     <t>The DAC institute</t>
+  </si>
+  <si>
+    <t>6d893451b8ed4159c9c31693894fdf6bb4e37c40705b977f315e00d75190d71e</t>
+  </si>
+  <si>
+    <t>1c9579c11d7e9eda0fd83beeb0d113e1d83af53aeba6747e251ebffbba0857a1</t>
+  </si>
+  <si>
+    <t>ac789d32d84025fd4f19f061d96279b719aaa8a92e7524aae00ec4d4a4d4c7b2</t>
+  </si>
+  <si>
+    <t>3451a704880381ece932362770fdfba9500970e3b61eac7e276cf832a696f6bc</t>
+  </si>
+  <si>
+    <t>2b5b7e057b3f29f65b81ce90e4d1f345989e82f0225dd0b688e3f7d17e188a5e</t>
+  </si>
+  <si>
+    <t>569792074549bd74dd021502bb8b93de93b2a020bebc36d85cb6860bd16523fd</t>
+  </si>
+  <si>
+    <t>6372bfee698058d7768ca8e051bff9f336dd0c6f256fad2802b89125b24be858</t>
+  </si>
+  <si>
+    <t>e830c31e41e4f210071b695eeab0672102d7ce4842d8f71ca4ff556661e767a9</t>
+  </si>
+  <si>
+    <t>f755b270ad22758bee88580199bc1edd8e0b5a366e0a49afbfe332753c7c65ff</t>
+  </si>
+  <si>
+    <t>98d69b3859d2ee3a6c047e64d75ff26081d1e01cc283dcffe7982034b5786c7c</t>
+  </si>
+  <si>
+    <t>ca8b627793c09722a8a67df9a86ca992d9c611da67f9e09dd82fa5fbbdfc888f</t>
+  </si>
+  <si>
+    <t>74473a16db3d3f037921fcb637c709a859f435ebb92acc13026dae56e82ce871</t>
+  </si>
+  <si>
+    <t>87915df7c6c014a380f9fded427b0650d15094b93b396e36f026ed8604ef29c2</t>
+  </si>
+  <si>
+    <t>61ea1a00a870846b7eb5af23a7d1642a12e0ae89dc0d8184ce01bc86641ba9e1</t>
+  </si>
+  <si>
+    <t>421a7518062f8620a046175510c42c27425bd39ee527c69eabdfde5b8cca21a8</t>
+  </si>
+  <si>
+    <t>31be4a412b08df968bfab48754cc87cc14a71c4a241110ad881eeee2e692c560</t>
+  </si>
+  <si>
+    <t>1aea8f7a679c57e09560176bd21e4b0c113f1975b8fe6452e312e23b780e7e04</t>
+  </si>
+  <si>
+    <t>acd38db5f1dd66f5360f09cf0b75917f840dd0cfae7c55de0ab5e78d254928ab</t>
+  </si>
+  <si>
+    <t>92a779a9456e487bcb6f64c37fe273d0d1e8ce63eaa04bffb1fe34e8f9ab1ca3</t>
+  </si>
+  <si>
+    <t>21168bff3d6d6427774100d1ebac454596d13e9ba8f9e532582ad61115d8dfb6</t>
+  </si>
+  <si>
+    <t>cbddfe7c8cc7d86036a9a89427b923b420618947c5b7e52cfad4f10637285d10</t>
+  </si>
+  <si>
+    <t>1adf6fe8f39577ba9ee04ecd54f7993171a38c4adf29af9e80479125dc125c7d</t>
+  </si>
+  <si>
+    <t>868f79790567d12c788da81e06fad6660dea7005a29d22113ece988cae6e3789</t>
+  </si>
+  <si>
+    <t>0aa199655fbcfd3210c6b1b6e448a5e6f550fab757020d00afab9da98d299f38</t>
+  </si>
+  <si>
+    <t>387528dc9007900d4c325d5f30c698b4e245cdceaafd6ede749e888f2c2d8b01</t>
+  </si>
+  <si>
+    <t>a5a665c7c9ac7869feefa638bc0c36c1277bf3806a5ca0dab6612a231b110c47</t>
+  </si>
+  <si>
+    <t>ff3407f770f6d8e3fd6deb58bea3812ebe7dc72a23530f83a9dc8b874b15678c</t>
+  </si>
+  <si>
+    <t>3bae81b1158274db6eb98914c45d35fa36dcd8a82436605fd036a371abf95d19</t>
+  </si>
+  <si>
+    <t>6d816fbfca7b79ce737b9ae2fc72ffb06b74fbcbf5fd1a572104eae2b1f87eea</t>
+  </si>
+  <si>
+    <t>c92b678b296e13393d96755fc4130bf567cb0ec76fc0c830cd5010c91fccf896</t>
+  </si>
+  <si>
+    <t>c464ca6e3fddb03069685ee61a16c02de708e114f5ed8c705c7c6feb974bdbcd</t>
+  </si>
+  <si>
+    <t>8cb0040d4e84f4f2c4f27a48d41864eb49f69719c2bb7e012e54cbf62d273692</t>
+  </si>
+  <si>
+    <t>9dea3f529fe2bf63657563630e9933a8883898ae449dd002b5eadf0031976909</t>
+  </si>
+  <si>
+    <t>6efad42ae46e2d2f9298ba8d206ae9490556b4ab204cf205106f5a6a5104c961</t>
+  </si>
+  <si>
+    <t>17e1149486c22e92abae2ff6534d9e2e0657f528aa96e0ecf24ab0164f484000</t>
+  </si>
+  <si>
+    <t>14e5353efad785d079a84e667398c4e47dca7769de5a8b4824b93039c02cc386</t>
+  </si>
+  <si>
+    <t>a3955d3579dfdb98c78d7eadab1045f2af24c311a679969d48944c5a7360d6c2</t>
+  </si>
+  <si>
+    <t>1cbec623ac2eec0e460433ce1b9d7dfe82f704a61ed2154d091865a38cb7f396</t>
+  </si>
+  <si>
+    <t>4024ee97fc733989e1f45a70c3afcbe14361f620a57af4f02c3e5f76befc2380</t>
+  </si>
+  <si>
+    <t>25b3ab9f971a12defb584e56f4e9bbe360c888f6025fc8b0fcbcf0075b522311</t>
+  </si>
+  <si>
+    <t>97d7d476e24a2d824259eda9877e22e8a40acd80b89e1f40cfd82567d9bc0fb5</t>
+  </si>
+  <si>
+    <t>a9e3af6a3f682dbf7aa672b46d293ae64da87829e7583d88e158c662b01c5e8d</t>
+  </si>
+  <si>
+    <t>f02e10ccabd47e0d1408d1b730b86f033b803ab7a8a3b244eaad8b190365decd</t>
+  </si>
+  <si>
+    <t>e09a51143ae290f7a914e36a045ce0cc1d9c388ea32bc2e33ba69cece7b069a7</t>
+  </si>
+  <si>
+    <t>07ce01d6f7b8d142e2b686fac6afce142ca969c763de623eedbfdbb72745746d</t>
+  </si>
+  <si>
+    <t>ad9938d9a42e0ae81035842ba7450026b9aa81299ce5fa733cdbd3597b47c317</t>
+  </si>
+  <si>
+    <t>7ac08879fca2f038419db2cd1617a124051a1da42a67875cda64b8a6c9b84c9a</t>
+  </si>
+  <si>
+    <t>f07649e2d937b32157f739f0d59dfc930336fb101f2004495a7827c1bd538409</t>
+  </si>
+  <si>
+    <t>cbd192a0bfc7deec6a1f7abadbea391eda38d1002f0b90e1dfb71dc4c965e647</t>
+  </si>
+  <si>
+    <t>9fa04196439164392c80761d8be02b6b3b5a573249fc0fcda42a795feb8e93f3</t>
+  </si>
+  <si>
+    <t>77d450e1497715383931c16df4180e8cc266678b30969884967cb938231cedc6</t>
+  </si>
+  <si>
+    <t>ba293f21da806db924a4d906641355dd6f6bb753dabbadd990fac7ec54150ceb</t>
   </si>
 </sst>
 </file>
@@ -9524,7 +9524,9 @@
   </sheetPr>
   <dimension ref="A1:I1006"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -9721,1498 +9723,1498 @@
         <v>91</v>
       </c>
       <c r="E7" s="6">
-        <v>92161</v>
+        <v>2049</v>
       </c>
       <c r="F7" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>199</v>
+      </c>
+      <c r="H7" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="G7" s="6" t="s">
-        <v>251</v>
-      </c>
-      <c r="H7" s="6" t="s">
+      <c r="I7" s="6" t="s">
         <v>93</v>
-      </c>
-      <c r="I7" s="6" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>87</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D8" s="6" t="s">
         <v>91</v>
       </c>
       <c r="E8" s="6">
-        <v>92161</v>
+        <v>6145</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>97</v>
+        <v>231</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>252</v>
+        <v>200</v>
       </c>
       <c r="H8" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="I8" s="6" t="s">
         <v>93</v>
-      </c>
-      <c r="I8" s="6" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>87</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>91</v>
       </c>
       <c r="E9" s="6">
-        <v>92161</v>
+        <v>4097</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>100</v>
+        <v>232</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>251</v>
+        <v>199</v>
       </c>
       <c r="H9" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="I9" s="6" t="s">
         <v>93</v>
-      </c>
-      <c r="I9" s="6" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>87</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="D10" s="6" t="s">
         <v>91</v>
       </c>
       <c r="E10" s="6">
-        <v>92161</v>
+        <v>6145</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>103</v>
+        <v>233</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>252</v>
+        <v>200</v>
       </c>
       <c r="H10" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="I10" s="6" t="s">
         <v>93</v>
-      </c>
-      <c r="I10" s="6" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>87</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="D11" s="6" t="s">
         <v>91</v>
       </c>
       <c r="E11" s="6">
-        <v>92161</v>
+        <v>6145</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>106</v>
+        <v>234</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>251</v>
+        <v>199</v>
       </c>
       <c r="H11" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="I11" s="6" t="s">
         <v>93</v>
-      </c>
-      <c r="I11" s="6" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>87</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="D12" s="6" t="s">
         <v>91</v>
       </c>
       <c r="E12" s="6">
-        <v>92161</v>
+        <v>8193</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>109</v>
+        <v>235</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>252</v>
+        <v>200</v>
       </c>
       <c r="H12" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="I12" s="6" t="s">
         <v>93</v>
-      </c>
-      <c r="I12" s="6" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>87</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="D13" s="6" t="s">
         <v>91</v>
       </c>
       <c r="E13" s="6">
-        <v>92161</v>
+        <v>4097</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>112</v>
+        <v>236</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>251</v>
+        <v>199</v>
       </c>
       <c r="H13" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="I13" s="6" t="s">
         <v>93</v>
-      </c>
-      <c r="I13" s="6" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="B14" s="6" t="s">
         <v>87</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="D14" s="6" t="s">
         <v>91</v>
       </c>
       <c r="E14" s="6">
-        <v>92161</v>
+        <v>4097</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>115</v>
+        <v>237</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>252</v>
+        <v>200</v>
       </c>
       <c r="H14" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="I14" s="6" t="s">
         <v>93</v>
-      </c>
-      <c r="I14" s="6" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="B15" s="6" t="s">
         <v>87</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="D15" s="6" t="s">
         <v>91</v>
       </c>
       <c r="E15" s="6">
-        <v>92161</v>
+        <v>2049</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>118</v>
+        <v>238</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>251</v>
+        <v>199</v>
       </c>
       <c r="H15" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="I15" s="6" t="s">
         <v>93</v>
-      </c>
-      <c r="I15" s="6" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="B16" s="6" t="s">
         <v>87</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="D16" s="6" t="s">
         <v>91</v>
       </c>
       <c r="E16" s="6">
-        <v>92161</v>
+        <v>8193</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>121</v>
+        <v>239</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>252</v>
+        <v>200</v>
       </c>
       <c r="H16" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="I16" s="6" t="s">
         <v>93</v>
-      </c>
-      <c r="I16" s="6" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="B17" s="6" t="s">
         <v>87</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
       <c r="D17" s="6" t="s">
         <v>91</v>
       </c>
       <c r="E17" s="6">
-        <v>92161</v>
+        <v>6145</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>124</v>
+        <v>240</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>251</v>
+        <v>199</v>
       </c>
       <c r="H17" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="I17" s="6" t="s">
         <v>93</v>
-      </c>
-      <c r="I17" s="6" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="s">
-        <v>125</v>
+        <v>114</v>
       </c>
       <c r="B18" s="6" t="s">
         <v>87</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>126</v>
+        <v>115</v>
       </c>
       <c r="D18" s="6" t="s">
         <v>91</v>
       </c>
       <c r="E18" s="6">
-        <v>92161</v>
+        <v>8193</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>127</v>
+        <v>241</v>
       </c>
       <c r="G18" s="6" t="s">
-        <v>252</v>
+        <v>200</v>
       </c>
       <c r="H18" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="I18" s="6" t="s">
         <v>93</v>
-      </c>
-      <c r="I18" s="6" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="6" t="s">
-        <v>128</v>
+        <v>116</v>
       </c>
       <c r="B19" s="6" t="s">
         <v>87</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>129</v>
+        <v>117</v>
       </c>
       <c r="D19" s="6" t="s">
         <v>91</v>
       </c>
       <c r="E19" s="6">
-        <v>92161</v>
+        <v>2049</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>130</v>
+        <v>242</v>
       </c>
       <c r="G19" s="6" t="s">
-        <v>251</v>
+        <v>199</v>
       </c>
       <c r="H19" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="I19" s="6" t="s">
         <v>93</v>
-      </c>
-      <c r="I19" s="6" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="6" t="s">
-        <v>131</v>
+        <v>118</v>
       </c>
       <c r="B20" s="6" t="s">
         <v>87</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>132</v>
+        <v>119</v>
       </c>
       <c r="D20" s="6" t="s">
         <v>91</v>
       </c>
       <c r="E20" s="6">
-        <v>92161</v>
+        <v>4097</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>133</v>
+        <v>243</v>
       </c>
       <c r="G20" s="6" t="s">
-        <v>252</v>
+        <v>200</v>
       </c>
       <c r="H20" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="I20" s="6" t="s">
         <v>93</v>
-      </c>
-      <c r="I20" s="6" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="6" t="s">
-        <v>134</v>
+        <v>120</v>
       </c>
       <c r="B21" s="6" t="s">
         <v>87</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>135</v>
+        <v>121</v>
       </c>
       <c r="D21" s="6" t="s">
         <v>91</v>
       </c>
       <c r="E21" s="6">
-        <v>92161</v>
+        <v>4097</v>
       </c>
       <c r="F21" s="6" t="s">
-        <v>136</v>
+        <v>244</v>
       </c>
       <c r="G21" s="6" t="s">
-        <v>251</v>
+        <v>199</v>
       </c>
       <c r="H21" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="I21" s="6" t="s">
         <v>93</v>
-      </c>
-      <c r="I21" s="6" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="6" t="s">
-        <v>137</v>
+        <v>122</v>
       </c>
       <c r="B22" s="6" t="s">
         <v>87</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>138</v>
+        <v>123</v>
       </c>
       <c r="D22" s="6" t="s">
         <v>91</v>
       </c>
       <c r="E22" s="6">
-        <v>92161</v>
+        <v>2049</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>139</v>
+        <v>245</v>
       </c>
       <c r="G22" s="6" t="s">
-        <v>252</v>
+        <v>200</v>
       </c>
       <c r="H22" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="I22" s="6" t="s">
         <v>93</v>
-      </c>
-      <c r="I22" s="6" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="6" t="s">
-        <v>140</v>
+        <v>124</v>
       </c>
       <c r="B23" s="6" t="s">
         <v>87</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>141</v>
+        <v>125</v>
       </c>
       <c r="D23" s="6" t="s">
         <v>91</v>
       </c>
       <c r="E23" s="6">
-        <v>92161</v>
+        <v>6145</v>
       </c>
       <c r="F23" s="6" t="s">
-        <v>142</v>
+        <v>246</v>
       </c>
       <c r="G23" s="6" t="s">
-        <v>251</v>
+        <v>199</v>
       </c>
       <c r="H23" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I23" s="6" t="s">
-        <v>143</v>
+        <v>126</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="6" t="s">
-        <v>144</v>
+        <v>127</v>
       </c>
       <c r="B24" s="6" t="s">
         <v>87</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>145</v>
+        <v>128</v>
       </c>
       <c r="D24" s="6" t="s">
         <v>91</v>
       </c>
       <c r="E24" s="6">
-        <v>92161</v>
+        <v>4097</v>
       </c>
       <c r="F24" s="6" t="s">
-        <v>146</v>
+        <v>247</v>
       </c>
       <c r="G24" s="6" t="s">
-        <v>252</v>
+        <v>200</v>
       </c>
       <c r="H24" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I24" s="6" t="s">
-        <v>143</v>
+        <v>126</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="6" t="s">
-        <v>147</v>
+        <v>129</v>
       </c>
       <c r="B25" s="6" t="s">
         <v>87</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>148</v>
+        <v>130</v>
       </c>
       <c r="D25" s="6" t="s">
         <v>91</v>
       </c>
       <c r="E25" s="6">
-        <v>92161</v>
+        <v>6145</v>
       </c>
       <c r="F25" s="6" t="s">
-        <v>149</v>
+        <v>248</v>
       </c>
       <c r="G25" s="6" t="s">
-        <v>251</v>
+        <v>199</v>
       </c>
       <c r="H25" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I25" s="6" t="s">
-        <v>143</v>
+        <v>126</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="6" t="s">
-        <v>150</v>
+        <v>131</v>
       </c>
       <c r="B26" s="6" t="s">
         <v>87</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>151</v>
+        <v>132</v>
       </c>
       <c r="D26" s="6" t="s">
         <v>91</v>
       </c>
       <c r="E26" s="6">
-        <v>92161</v>
+        <v>8193</v>
       </c>
       <c r="F26" s="6" t="s">
-        <v>152</v>
+        <v>249</v>
       </c>
       <c r="G26" s="6" t="s">
-        <v>252</v>
+        <v>200</v>
       </c>
       <c r="H26" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I26" s="6" t="s">
-        <v>143</v>
+        <v>126</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="6" t="s">
-        <v>153</v>
+        <v>133</v>
       </c>
       <c r="B27" s="6" t="s">
         <v>87</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>154</v>
+        <v>134</v>
       </c>
       <c r="D27" s="6" t="s">
         <v>91</v>
       </c>
       <c r="E27" s="6">
-        <v>92161</v>
+        <v>6145</v>
       </c>
       <c r="F27" s="6" t="s">
-        <v>155</v>
+        <v>250</v>
       </c>
       <c r="G27" s="6" t="s">
-        <v>251</v>
+        <v>199</v>
       </c>
       <c r="H27" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I27" s="6" t="s">
-        <v>143</v>
+        <v>126</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="6" t="s">
-        <v>156</v>
+        <v>135</v>
       </c>
       <c r="B28" s="6" t="s">
         <v>87</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>157</v>
+        <v>136</v>
       </c>
       <c r="D28" s="6" t="s">
         <v>91</v>
       </c>
       <c r="E28" s="6">
-        <v>92161</v>
+        <v>8193</v>
       </c>
       <c r="F28" s="6" t="s">
-        <v>158</v>
+        <v>251</v>
       </c>
       <c r="G28" s="6" t="s">
-        <v>252</v>
+        <v>200</v>
       </c>
       <c r="H28" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I28" s="6" t="s">
-        <v>143</v>
+        <v>126</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" s="6" t="s">
-        <v>159</v>
+        <v>137</v>
       </c>
       <c r="B29" s="6" t="s">
         <v>87</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>160</v>
+        <v>138</v>
       </c>
       <c r="D29" s="6" t="s">
         <v>91</v>
       </c>
       <c r="E29" s="6">
-        <v>92161</v>
+        <v>4097</v>
       </c>
       <c r="F29" s="6" t="s">
-        <v>161</v>
+        <v>252</v>
       </c>
       <c r="G29" s="6" t="s">
-        <v>251</v>
+        <v>199</v>
       </c>
       <c r="H29" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I29" s="6" t="s">
-        <v>162</v>
+        <v>139</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" s="6" t="s">
-        <v>163</v>
+        <v>140</v>
       </c>
       <c r="B30" s="6" t="s">
         <v>87</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>164</v>
+        <v>141</v>
       </c>
       <c r="D30" s="6" t="s">
         <v>91</v>
       </c>
       <c r="E30" s="6">
-        <v>92161</v>
+        <v>8193</v>
       </c>
       <c r="F30" s="6" t="s">
-        <v>165</v>
+        <v>253</v>
       </c>
       <c r="G30" s="6" t="s">
-        <v>252</v>
+        <v>200</v>
       </c>
       <c r="H30" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I30" s="6" t="s">
-        <v>162</v>
+        <v>139</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" s="6" t="s">
-        <v>166</v>
+        <v>142</v>
       </c>
       <c r="B31" s="6" t="s">
         <v>88</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>167</v>
+        <v>143</v>
       </c>
       <c r="D31" s="6" t="s">
         <v>91</v>
       </c>
       <c r="E31" s="6">
-        <v>92161</v>
+        <v>8193</v>
       </c>
       <c r="F31" s="6" t="s">
-        <v>168</v>
+        <v>254</v>
       </c>
       <c r="G31" s="6" t="s">
-        <v>251</v>
+        <v>199</v>
       </c>
       <c r="H31" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I31" s="6" t="s">
-        <v>162</v>
+        <v>139</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" s="6" t="s">
-        <v>169</v>
+        <v>144</v>
       </c>
       <c r="B32" s="6" t="s">
         <v>88</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>170</v>
+        <v>145</v>
       </c>
       <c r="D32" s="6" t="s">
         <v>91</v>
       </c>
       <c r="E32" s="6">
-        <v>92161</v>
+        <v>8193</v>
       </c>
       <c r="F32" s="6" t="s">
-        <v>171</v>
+        <v>255</v>
       </c>
       <c r="G32" s="6" t="s">
-        <v>252</v>
+        <v>200</v>
       </c>
       <c r="H32" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I32" s="6" t="s">
-        <v>162</v>
+        <v>139</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" s="6" t="s">
-        <v>172</v>
+        <v>146</v>
       </c>
       <c r="B33" s="6" t="s">
         <v>88</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>173</v>
+        <v>147</v>
       </c>
       <c r="D33" s="6" t="s">
         <v>91</v>
       </c>
       <c r="E33" s="6">
-        <v>92161</v>
+        <v>4097</v>
       </c>
       <c r="F33" s="6" t="s">
-        <v>174</v>
+        <v>256</v>
       </c>
       <c r="G33" s="6" t="s">
-        <v>251</v>
+        <v>199</v>
       </c>
       <c r="H33" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I33" s="6" t="s">
-        <v>162</v>
+        <v>139</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" s="6" t="s">
-        <v>175</v>
+        <v>148</v>
       </c>
       <c r="B34" s="6" t="s">
         <v>88</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>176</v>
+        <v>149</v>
       </c>
       <c r="D34" s="6" t="s">
         <v>91</v>
       </c>
       <c r="E34" s="6">
-        <v>92161</v>
+        <v>4097</v>
       </c>
       <c r="F34" s="6" t="s">
-        <v>177</v>
+        <v>257</v>
       </c>
       <c r="G34" s="6" t="s">
-        <v>252</v>
+        <v>200</v>
       </c>
       <c r="H34" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I34" s="6" t="s">
-        <v>162</v>
+        <v>139</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" s="6" t="s">
-        <v>178</v>
+        <v>150</v>
       </c>
       <c r="B35" s="6" t="s">
         <v>88</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>179</v>
+        <v>151</v>
       </c>
       <c r="D35" s="6" t="s">
         <v>91</v>
       </c>
       <c r="E35" s="6">
-        <v>92161</v>
+        <v>2049</v>
       </c>
       <c r="F35" s="6" t="s">
-        <v>180</v>
+        <v>258</v>
       </c>
       <c r="G35" s="6" t="s">
-        <v>251</v>
+        <v>199</v>
       </c>
       <c r="H35" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I35" s="6" t="s">
-        <v>162</v>
+        <v>139</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" s="6" t="s">
-        <v>181</v>
+        <v>152</v>
       </c>
       <c r="B36" s="6" t="s">
         <v>88</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>182</v>
+        <v>153</v>
       </c>
       <c r="D36" s="6" t="s">
         <v>91</v>
       </c>
       <c r="E36" s="6">
-        <v>92161</v>
+        <v>6145</v>
       </c>
       <c r="F36" s="6" t="s">
-        <v>183</v>
+        <v>259</v>
       </c>
       <c r="G36" s="6" t="s">
-        <v>252</v>
+        <v>200</v>
       </c>
       <c r="H36" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I36" s="6" t="s">
-        <v>162</v>
+        <v>139</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" s="6" t="s">
-        <v>184</v>
+        <v>154</v>
       </c>
       <c r="B37" s="6" t="s">
         <v>88</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>185</v>
+        <v>155</v>
       </c>
       <c r="D37" s="6" t="s">
         <v>91</v>
       </c>
       <c r="E37" s="6">
-        <v>92161</v>
+        <v>6145</v>
       </c>
       <c r="F37" s="6" t="s">
-        <v>186</v>
+        <v>260</v>
       </c>
       <c r="G37" s="6" t="s">
-        <v>251</v>
+        <v>199</v>
       </c>
       <c r="H37" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I37" s="6" t="s">
-        <v>162</v>
+        <v>139</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" s="6" t="s">
-        <v>187</v>
+        <v>156</v>
       </c>
       <c r="B38" s="6" t="s">
         <v>88</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>188</v>
+        <v>157</v>
       </c>
       <c r="D38" s="6" t="s">
         <v>91</v>
       </c>
       <c r="E38" s="6">
-        <v>92161</v>
+        <v>2049</v>
       </c>
       <c r="F38" s="6" t="s">
-        <v>189</v>
+        <v>261</v>
       </c>
       <c r="G38" s="6" t="s">
-        <v>252</v>
+        <v>200</v>
       </c>
       <c r="H38" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I38" s="6" t="s">
-        <v>162</v>
+        <v>139</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" s="6" t="s">
-        <v>190</v>
+        <v>158</v>
       </c>
       <c r="B39" s="6" t="s">
         <v>88</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>191</v>
+        <v>159</v>
       </c>
       <c r="D39" s="6" t="s">
         <v>91</v>
       </c>
       <c r="E39" s="6">
-        <v>92161</v>
+        <v>8193</v>
       </c>
       <c r="F39" s="6" t="s">
-        <v>192</v>
+        <v>262</v>
       </c>
       <c r="G39" s="6" t="s">
-        <v>251</v>
+        <v>199</v>
       </c>
       <c r="H39" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I39" s="6" t="s">
-        <v>162</v>
+        <v>139</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" s="6" t="s">
-        <v>193</v>
+        <v>160</v>
       </c>
       <c r="B40" s="6" t="s">
         <v>88</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>194</v>
+        <v>161</v>
       </c>
       <c r="D40" s="6" t="s">
         <v>91</v>
       </c>
       <c r="E40" s="6">
-        <v>92161</v>
+        <v>8193</v>
       </c>
       <c r="F40" s="6" t="s">
-        <v>195</v>
+        <v>263</v>
       </c>
       <c r="G40" s="6" t="s">
-        <v>252</v>
+        <v>200</v>
       </c>
       <c r="H40" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I40" s="6" t="s">
-        <v>162</v>
+        <v>139</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" s="6" t="s">
-        <v>196</v>
+        <v>162</v>
       </c>
       <c r="B41" s="6" t="s">
         <v>88</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>197</v>
+        <v>163</v>
       </c>
       <c r="D41" s="6" t="s">
         <v>91</v>
       </c>
       <c r="E41" s="6">
-        <v>92161</v>
-      </c>
-      <c r="F41" s="6" t="s">
-        <v>198</v>
+        <v>8193</v>
+      </c>
+      <c r="F41" s="16" t="s">
+        <v>264</v>
       </c>
       <c r="G41" s="6" t="s">
-        <v>251</v>
+        <v>199</v>
       </c>
       <c r="H41" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I41" s="6" t="s">
-        <v>162</v>
+        <v>139</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" s="6" t="s">
-        <v>199</v>
+        <v>164</v>
       </c>
       <c r="B42" s="6" t="s">
         <v>88</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>200</v>
+        <v>165</v>
       </c>
       <c r="D42" s="6" t="s">
         <v>91</v>
       </c>
       <c r="E42" s="6">
-        <v>92161</v>
-      </c>
-      <c r="F42" s="6" t="s">
-        <v>201</v>
+        <v>6145</v>
+      </c>
+      <c r="F42" s="16" t="s">
+        <v>265</v>
       </c>
       <c r="G42" s="6" t="s">
-        <v>252</v>
+        <v>200</v>
       </c>
       <c r="H42" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I42" s="6" t="s">
-        <v>162</v>
+        <v>139</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" s="6" t="s">
-        <v>202</v>
+        <v>166</v>
       </c>
       <c r="B43" s="6" t="s">
         <v>88</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>203</v>
+        <v>167</v>
       </c>
       <c r="D43" s="6" t="s">
         <v>91</v>
       </c>
       <c r="E43" s="6">
-        <v>92161</v>
+        <v>4097</v>
       </c>
       <c r="F43" s="6" t="s">
-        <v>204</v>
+        <v>266</v>
       </c>
       <c r="G43" s="6" t="s">
-        <v>251</v>
+        <v>199</v>
       </c>
       <c r="H43" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I43" s="6" t="s">
-        <v>162</v>
+        <v>139</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" s="6" t="s">
-        <v>205</v>
+        <v>168</v>
       </c>
       <c r="B44" s="6" t="s">
         <v>88</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>206</v>
+        <v>169</v>
       </c>
       <c r="D44" s="6" t="s">
         <v>91</v>
       </c>
       <c r="E44" s="6">
-        <v>92161</v>
+        <v>2049</v>
       </c>
       <c r="F44" s="6" t="s">
-        <v>207</v>
+        <v>267</v>
       </c>
       <c r="G44" s="6" t="s">
-        <v>252</v>
+        <v>200</v>
       </c>
       <c r="H44" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I44" s="6" t="s">
-        <v>162</v>
+        <v>139</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" s="6" t="s">
-        <v>208</v>
+        <v>170</v>
       </c>
       <c r="B45" s="6" t="s">
         <v>88</v>
       </c>
       <c r="C45" s="6" t="s">
-        <v>209</v>
+        <v>171</v>
       </c>
       <c r="D45" s="6" t="s">
         <v>91</v>
       </c>
       <c r="E45" s="6">
-        <v>92161</v>
+        <v>6145</v>
       </c>
       <c r="F45" s="6" t="s">
-        <v>210</v>
+        <v>268</v>
       </c>
       <c r="G45" s="6" t="s">
-        <v>251</v>
+        <v>199</v>
       </c>
       <c r="H45" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I45" s="6" t="s">
-        <v>162</v>
+        <v>139</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" s="6" t="s">
-        <v>211</v>
+        <v>172</v>
       </c>
       <c r="B46" s="6" t="s">
         <v>88</v>
       </c>
       <c r="C46" s="6" t="s">
-        <v>212</v>
+        <v>173</v>
       </c>
       <c r="D46" s="6" t="s">
         <v>91</v>
       </c>
       <c r="E46" s="6">
-        <v>92161</v>
+        <v>8193</v>
       </c>
       <c r="F46" s="6" t="s">
-        <v>213</v>
+        <v>269</v>
       </c>
       <c r="G46" s="6" t="s">
-        <v>252</v>
+        <v>200</v>
       </c>
       <c r="H46" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I46" s="6" t="s">
-        <v>162</v>
+        <v>139</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" s="6" t="s">
-        <v>214</v>
+        <v>174</v>
       </c>
       <c r="B47" s="6" t="s">
         <v>88</v>
       </c>
       <c r="C47" s="6" t="s">
-        <v>215</v>
+        <v>175</v>
       </c>
       <c r="D47" s="6" t="s">
         <v>91</v>
       </c>
       <c r="E47" s="6">
-        <v>92161</v>
+        <v>4097</v>
       </c>
       <c r="F47" s="6" t="s">
-        <v>216</v>
+        <v>270</v>
       </c>
       <c r="G47" s="6" t="s">
-        <v>251</v>
+        <v>199</v>
       </c>
       <c r="H47" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I47" s="6" t="s">
-        <v>162</v>
+        <v>139</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" s="6" t="s">
-        <v>217</v>
+        <v>176</v>
       </c>
       <c r="B48" s="6" t="s">
         <v>88</v>
       </c>
       <c r="C48" s="6" t="s">
-        <v>218</v>
+        <v>177</v>
       </c>
       <c r="D48" s="6" t="s">
         <v>91</v>
       </c>
       <c r="E48" s="6">
-        <v>92161</v>
+        <v>6145</v>
       </c>
       <c r="F48" s="6" t="s">
-        <v>219</v>
+        <v>271</v>
       </c>
       <c r="G48" s="6" t="s">
-        <v>252</v>
+        <v>200</v>
       </c>
       <c r="H48" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I48" s="6" t="s">
-        <v>162</v>
+        <v>139</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" s="6" t="s">
-        <v>220</v>
+        <v>178</v>
       </c>
       <c r="B49" s="6" t="s">
         <v>88</v>
       </c>
       <c r="C49" s="6" t="s">
-        <v>221</v>
+        <v>179</v>
       </c>
       <c r="D49" s="6" t="s">
         <v>91</v>
       </c>
       <c r="E49" s="6">
-        <v>92161</v>
+        <v>8193</v>
       </c>
       <c r="F49" s="6" t="s">
-        <v>222</v>
+        <v>272</v>
       </c>
       <c r="G49" s="6" t="s">
-        <v>251</v>
+        <v>199</v>
       </c>
       <c r="H49" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I49" s="6" t="s">
-        <v>223</v>
+        <v>180</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50" s="6" t="s">
-        <v>224</v>
+        <v>181</v>
       </c>
       <c r="B50" s="6" t="s">
         <v>88</v>
       </c>
       <c r="C50" s="6" t="s">
-        <v>225</v>
+        <v>182</v>
       </c>
       <c r="D50" s="6" t="s">
         <v>91</v>
       </c>
       <c r="E50" s="6">
-        <v>92161</v>
+        <v>4097</v>
       </c>
       <c r="F50" s="6" t="s">
-        <v>226</v>
+        <v>273</v>
       </c>
       <c r="G50" s="6" t="s">
-        <v>252</v>
+        <v>200</v>
       </c>
       <c r="H50" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I50" s="6" t="s">
-        <v>223</v>
+        <v>180</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51" s="6" t="s">
-        <v>227</v>
+        <v>183</v>
       </c>
       <c r="B51" s="6" t="s">
         <v>88</v>
       </c>
       <c r="C51" s="6" t="s">
-        <v>228</v>
+        <v>184</v>
       </c>
       <c r="D51" s="6" t="s">
         <v>91</v>
       </c>
       <c r="E51" s="6">
-        <v>92161</v>
+        <v>8193</v>
       </c>
       <c r="F51" s="6" t="s">
-        <v>229</v>
+        <v>274</v>
       </c>
       <c r="G51" s="6" t="s">
-        <v>251</v>
+        <v>199</v>
       </c>
       <c r="H51" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I51" s="6" t="s">
-        <v>223</v>
+        <v>180</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A52" s="6" t="s">
-        <v>230</v>
+        <v>185</v>
       </c>
       <c r="B52" s="6" t="s">
         <v>88</v>
       </c>
       <c r="C52" s="6" t="s">
-        <v>231</v>
+        <v>186</v>
       </c>
       <c r="D52" s="6" t="s">
         <v>91</v>
       </c>
       <c r="E52" s="6">
-        <v>92161</v>
+        <v>6145</v>
       </c>
       <c r="F52" s="6" t="s">
-        <v>232</v>
+        <v>275</v>
       </c>
       <c r="G52" s="6" t="s">
-        <v>252</v>
+        <v>200</v>
       </c>
       <c r="H52" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I52" s="6" t="s">
-        <v>223</v>
+        <v>180</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A53" s="6" t="s">
-        <v>233</v>
+        <v>187</v>
       </c>
       <c r="B53" s="6" t="s">
         <v>88</v>
       </c>
       <c r="C53" s="6" t="s">
-        <v>234</v>
+        <v>188</v>
       </c>
       <c r="D53" s="6" t="s">
         <v>91</v>
       </c>
       <c r="E53" s="6">
-        <v>92161</v>
+        <v>6145</v>
       </c>
       <c r="F53" s="6" t="s">
-        <v>235</v>
+        <v>276</v>
       </c>
       <c r="G53" s="6" t="s">
-        <v>251</v>
+        <v>199</v>
       </c>
       <c r="H53" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I53" s="6" t="s">
-        <v>223</v>
+        <v>180</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A54" s="6" t="s">
-        <v>236</v>
+        <v>189</v>
       </c>
       <c r="B54" s="6" t="s">
         <v>88</v>
       </c>
       <c r="C54" s="6" t="s">
-        <v>237</v>
+        <v>190</v>
       </c>
       <c r="D54" s="6" t="s">
         <v>91</v>
       </c>
       <c r="E54" s="6">
-        <v>92161</v>
+        <v>8193</v>
       </c>
       <c r="F54" s="16" t="s">
-        <v>238</v>
+        <v>277</v>
       </c>
       <c r="G54" s="6" t="s">
-        <v>252</v>
+        <v>200</v>
       </c>
       <c r="H54" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I54" s="6" t="s">
-        <v>223</v>
+        <v>180</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A55" s="6" t="s">
-        <v>239</v>
+        <v>191</v>
       </c>
       <c r="B55" s="6" t="s">
         <v>88</v>
       </c>
       <c r="C55" s="6" t="s">
-        <v>240</v>
+        <v>192</v>
       </c>
       <c r="D55" s="6" t="s">
         <v>91</v>
       </c>
       <c r="E55" s="6">
-        <v>92161</v>
+        <v>4097</v>
       </c>
       <c r="F55" s="6" t="s">
-        <v>241</v>
+        <v>278</v>
       </c>
       <c r="G55" s="6" t="s">
-        <v>251</v>
+        <v>199</v>
       </c>
       <c r="H55" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I55" s="6" t="s">
-        <v>223</v>
+        <v>180</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A56" s="6" t="s">
-        <v>242</v>
+        <v>193</v>
       </c>
       <c r="B56" s="6" t="s">
         <v>88</v>
       </c>
       <c r="C56" s="6" t="s">
-        <v>243</v>
+        <v>194</v>
       </c>
       <c r="D56" s="6" t="s">
         <v>91</v>
       </c>
       <c r="E56" s="6">
-        <v>92161</v>
+        <v>4097</v>
       </c>
       <c r="F56" s="6" t="s">
-        <v>244</v>
+        <v>279</v>
       </c>
       <c r="G56" s="6" t="s">
-        <v>252</v>
+        <v>200</v>
       </c>
       <c r="H56" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I56" s="6" t="s">
-        <v>223</v>
+        <v>180</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A57" s="6" t="s">
-        <v>245</v>
+        <v>195</v>
       </c>
       <c r="B57" s="6" t="s">
         <v>88</v>
       </c>
       <c r="C57" s="6" t="s">
-        <v>246</v>
+        <v>196</v>
       </c>
       <c r="D57" s="6" t="s">
         <v>91</v>
       </c>
       <c r="E57" s="6">
-        <v>92161</v>
+        <v>8193</v>
       </c>
       <c r="F57" s="6" t="s">
-        <v>247</v>
+        <v>280</v>
       </c>
       <c r="G57" s="6" t="s">
-        <v>251</v>
+        <v>199</v>
       </c>
       <c r="H57" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I57" s="6" t="s">
-        <v>223</v>
+        <v>180</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A58" s="6" t="s">
-        <v>248</v>
+        <v>197</v>
       </c>
       <c r="B58" s="6" t="s">
         <v>88</v>
       </c>
       <c r="C58" s="6" t="s">
-        <v>249</v>
+        <v>198</v>
       </c>
       <c r="D58" s="6" t="s">
         <v>91</v>
       </c>
       <c r="E58" s="6">
-        <v>92161</v>
+        <v>6145</v>
       </c>
       <c r="F58" s="6" t="s">
-        <v>250</v>
+        <v>281</v>
       </c>
       <c r="G58" s="6" t="s">
-        <v>252</v>
+        <v>200</v>
       </c>
       <c r="H58" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I58" s="6" t="s">
-        <v>223</v>
+        <v>180</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.2">
@@ -21766,70 +21768,70 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>253</v>
+        <v>201</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>254</v>
+        <v>202</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>255</v>
+        <v>203</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>256</v>
+        <v>204</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="9" t="s">
-        <v>143</v>
+        <v>126</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>257</v>
+        <v>205</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>258</v>
+        <v>206</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>259</v>
+        <v>207</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>256</v>
+        <v>204</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="9" t="s">
-        <v>162</v>
+        <v>139</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>260</v>
+        <v>208</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>261</v>
+        <v>209</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>262</v>
+        <v>210</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>256</v>
+        <v>204</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="9" t="s">
-        <v>223</v>
+        <v>180</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>263</v>
+        <v>211</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>264</v>
+        <v>212</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>265</v>
+        <v>213</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>266</v>
+        <v>214</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -28981,54 +28983,54 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
-        <v>256</v>
+        <v>204</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>267</v>
+        <v>215</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>268</v>
+        <v>216</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>269</v>
+        <v>217</v>
       </c>
       <c r="E7" s="17" t="s">
-        <v>270</v>
+        <v>218</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>271</v>
+        <v>219</v>
       </c>
       <c r="G7" s="12" t="s">
-        <v>272</v>
+        <v>220</v>
       </c>
       <c r="H7" s="12" t="s">
-        <v>273</v>
+        <v>221</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
-        <v>266</v>
+        <v>214</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>274</v>
+        <v>222</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>275</v>
+        <v>223</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>276</v>
+        <v>224</v>
       </c>
       <c r="E8" s="17" t="s">
-        <v>277</v>
+        <v>225</v>
       </c>
       <c r="F8" s="12" t="s">
-        <v>271</v>
+        <v>219</v>
       </c>
       <c r="G8" s="12" t="s">
-        <v>278</v>
+        <v>226</v>
       </c>
       <c r="H8" s="12" t="s">
-        <v>279</v>
+        <v>227</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
@@ -39102,13 +39104,13 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="15" t="s">
-        <v>271</v>
+        <v>219</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>280</v>
+        <v>228</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>281</v>
+        <v>229</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Add non-zero file content (#9)
* Add non-zero file content

* Slightly enlarge minimal_1 filesizes and move filename content to
beginning
</commit_message>
<xml_diff>
--- a/minimal_1/metadata.xlsx
+++ b/minimal_1/metadata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/dev/example-data/minimal_1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{940C727C-6C82-6040-8232-F5EA0245E7F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFA2D7B8-8CE6-1146-9BEF-A124E6ECA0F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="27300" windowHeight="28300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -317,9 +317,6 @@
     <t>FASTQ</t>
   </si>
   <si>
-    <t>07611c4987b9e5be1304a992dbc25242824acf808c829819732a8f5f6c40e731</t>
-  </si>
-  <si>
     <t>SHA256</t>
   </si>
   <si>
@@ -332,16 +329,10 @@
     <t>SEQ_FILE_A_R2.fastq.gz</t>
   </si>
   <si>
-    <t>ba7f0fa2da3c1bd473b01985c2fd25175d55f1edb27e530d735ff85ed187c122</t>
-  </si>
-  <si>
     <t>FILE_3</t>
   </si>
   <si>
     <t>SEQ_FILE_B_R1.fastq.gz</t>
-  </si>
-  <si>
-    <t>cbfa35d3a7d83b4ae5e3b06b04f3d784f2094497d434c9e6b50ac36753ee0025</t>
   </si>
   <si>
     <t>FILE_4</t>
@@ -350,16 +341,10 @@
     <t>SEQ_FILE_B_R2.fastq.gz</t>
   </si>
   <si>
-    <t>d42f211b7c589961332f86a2a41945ef9f3dd8ffc01a34d7755c27f7eb5b0bdb</t>
-  </si>
-  <si>
     <t>FILE_5</t>
   </si>
   <si>
     <t>SEQ_FILE_C_R1.fastq.gz</t>
-  </si>
-  <si>
-    <t>299585554663327257bd92a624760a3cbb009804a910ba03fc977d297d62ec7f</t>
   </si>
   <si>
     <t>FILE_6</t>
@@ -368,16 +353,10 @@
     <t>SEQ_FILE_C_R2.fastq.gz</t>
   </si>
   <si>
-    <t>83b23fb63eaa7dd8fed5447cc719077412bcb7cd5a82e710bae56643c00f27a2</t>
-  </si>
-  <si>
     <t>FILE_7</t>
   </si>
   <si>
     <t>SEQ_FILE_D_R1.fastq.gz</t>
-  </si>
-  <si>
-    <t>35f68cc8abc534f8ccb7e827aa4ab0f5d3736c310701144217e433af86c2f132</t>
   </si>
   <si>
     <t>FILE_8</t>
@@ -386,16 +365,10 @@
     <t>SEQ_FILE_D_R2.fastq.gz</t>
   </si>
   <si>
-    <t>05d1ed4457580cafab18e3cc06c8cac3bd1c6def191704e70c7e11d221b69f12</t>
-  </si>
-  <si>
     <t>FILE_9</t>
   </si>
   <si>
     <t>SEQ_FILE_E_R1.fastq.gz</t>
-  </si>
-  <si>
-    <t>cd230d8cf3bcdd10292a54cccc5c168dfec1d51b416ddc5102cbea259f3562bd</t>
   </si>
   <si>
     <t>FILE_10</t>
@@ -404,16 +377,10 @@
     <t>SEQ_FILE_E_R2.fastq.gz</t>
   </si>
   <si>
-    <t>7bdf0cb577c4b08a0890ece353a287493ea46c1fd8a2f9e27cb267be8c89c06c</t>
-  </si>
-  <si>
     <t>FILE_11</t>
   </si>
   <si>
     <t>SEQ_FILE_F_R1.fastq.gz</t>
-  </si>
-  <si>
-    <t>e383dd77d2e758d6373bff3abf501011fe6fb5c7af3089fd27abf367d4a92df9</t>
   </si>
   <si>
     <t>FILE_12</t>
@@ -422,16 +389,10 @@
     <t>SEQ_FILE_F_R2.fastq.gz</t>
   </si>
   <si>
-    <t>7729bc30f812e9ec967f89b3a1ad96f9290ffb92148baed608f520137a9fcff2</t>
-  </si>
-  <si>
     <t>FILE_13</t>
   </si>
   <si>
     <t>SEQ_FILE_G_R1.fastq.gz</t>
-  </si>
-  <si>
-    <t>e4bdbee6ace3161310e2b2f1eb16486509c6152f75f8c4da6d255289cd463943</t>
   </si>
   <si>
     <t>FILE_14</t>
@@ -440,16 +401,10 @@
     <t>SEQ_FILE_G_R2.fastq.gz</t>
   </si>
   <si>
-    <t>1dd5ca9bff0f1a48ee4c423a07cb7fd4e53c4c253d9e6d389e35d3be3e215e4e</t>
-  </si>
-  <si>
     <t>FILE_15</t>
   </si>
   <si>
     <t>SEQ_FILE_H_R1.fastq.gz</t>
-  </si>
-  <si>
-    <t>8d214cc1d2556bc6111de52e785ca1cde68b0fb024da219841552e328351ff3b</t>
   </si>
   <si>
     <t>FILE_16</t>
@@ -458,16 +413,10 @@
     <t>SEQ_FILE_H_R2.fastq.gz</t>
   </si>
   <si>
-    <t>358599ff0a1f1f15ce42b484496bc8dafb66ac07f2ab55ba0e2482e191ca5747</t>
-  </si>
-  <si>
     <t>FILE_17</t>
   </si>
   <si>
     <t>SEQ_FILE_I_R1.fastq.gz</t>
-  </si>
-  <si>
-    <t>b7fd9aca6c35f44baab8a8f750049620c5ccff3b4ce300ff9a282682a7302a65</t>
   </si>
   <si>
     <t>DS_2</t>
@@ -479,16 +428,10 @@
     <t>SEQ_FILE_I_R2.fastq.gz</t>
   </si>
   <si>
-    <t>2f660b9617185b44d2ec186eaf6299a43e8860a986077f9961e6ed87fea64824</t>
-  </si>
-  <si>
     <t>FILE_19</t>
   </si>
   <si>
     <t>SEQ_FILE_J_R1.fastq.gz</t>
-  </si>
-  <si>
-    <t>fec3b1b125f5270ff644c7e197494e8f0f20d8d5666065891cdfa3a9b6afd088</t>
   </si>
   <si>
     <t>FILE_20</t>
@@ -497,16 +440,10 @@
     <t>SEQ_FILE_J_R2.fastq.gz</t>
   </si>
   <si>
-    <t>03aa21f81b69d9484d58d9fcd7b6f10f3c2921d02034053fd89746742d0b48db</t>
-  </si>
-  <si>
     <t>FILE_21</t>
   </si>
   <si>
     <t>SEQ_FILE_K_R1.fastq.gz</t>
-  </si>
-  <si>
-    <t>96a4fe6942d341f74d18bd1c9d02e4af3327e18242591434024101dceafc6d4c</t>
   </si>
   <si>
     <t>FILE_22</t>
@@ -515,16 +452,10 @@
     <t>SEQ_FILE_K_R2.fastq.gz</t>
   </si>
   <si>
-    <t>4f8b52e0e874bfe1ae8813cbde44a102b85462f4ffb95c08f147771d0d5a5ae5</t>
-  </si>
-  <si>
     <t>FILE_23</t>
   </si>
   <si>
     <t>SEQ_FILE_L_R1.fastq.gz</t>
-  </si>
-  <si>
-    <t>a65dca5defc93dea1164839398df8a01a32370234a35a146a78018c2155c3b04</t>
   </si>
   <si>
     <t>DS_3</t>
@@ -536,16 +467,10 @@
     <t>SEQ_FILE_L_R2.fastq.gz</t>
   </si>
   <si>
-    <t>f42fa32c6bae7d38e4fe613fcca2f82952ffcb88d422bc2271bcb07bdbc51d9c</t>
-  </si>
-  <si>
     <t>FILE_25</t>
   </si>
   <si>
     <t>SEQ_FILE_M_R1.fastq.gz</t>
-  </si>
-  <si>
-    <t>6aa0b2825179a9998f78b11dcefefde944e21d7f45ee71a4e998ee9b94fc6ed4</t>
   </si>
   <si>
     <t>FILE_26</t>
@@ -554,16 +479,10 @@
     <t>SEQ_FILE_M_R2.fastq.gz</t>
   </si>
   <si>
-    <t>82f8ef5f7bd14703ca7e8a63f7bd10b9910bb195dc7fefdeb86794078a809d5e</t>
-  </si>
-  <si>
     <t>FILE_27</t>
   </si>
   <si>
     <t>SEQ_FILE_N_R1.fastq.gz</t>
-  </si>
-  <si>
-    <t>b25f7ae42b96cd6f0ad2bd797ae3a7e53e7e662786f2ffe1fe6bb1a8dfe7096b</t>
   </si>
   <si>
     <t>FILE_28</t>
@@ -572,16 +491,10 @@
     <t>SEQ_FILE_N_R2.fastq.gz</t>
   </si>
   <si>
-    <t>82be207843fb30084226cea0ae64e8247f84b4592a6b3539aa756dd871b54f96</t>
-  </si>
-  <si>
     <t>FILE_29</t>
   </si>
   <si>
     <t>SEQ_FILE_O_R1.fastq.gz</t>
-  </si>
-  <si>
-    <t>40a64a7c104f67ccf6521af0d25644c0adf270db11e322172a19e5576f9e9db7</t>
   </si>
   <si>
     <t>FILE_30</t>
@@ -590,16 +503,10 @@
     <t>SEQ_FILE_O_R2.fastq.gz</t>
   </si>
   <si>
-    <t>0b0663e0391b1d2b3b513be5981030a5b34337c4cfb4b978bfa07e04f48ecfe9</t>
-  </si>
-  <si>
     <t>FILE_31</t>
   </si>
   <si>
     <t>SEQ_FILE_P_R1.fastq.gz</t>
-  </si>
-  <si>
-    <t>ec8d0dfd3815bd2d2db636432d9d5471522a8b34c8429728e67319672f0e293f</t>
   </si>
   <si>
     <t>FILE_32</t>
@@ -608,16 +515,10 @@
     <t>SEQ_FILE_P_R2.fastq.gz</t>
   </si>
   <si>
-    <t>30439ff89fe2b9a373fcaac3c8bb1bfa912381c675d7663112ee922768170f8e</t>
-  </si>
-  <si>
     <t>FILE_33</t>
   </si>
   <si>
     <t>SEQ_FILE_Q_R1.fastq.gz</t>
-  </si>
-  <si>
-    <t>f54a61941105b510acafd91f9392efd5a3d8cc7f965960983e0cbfe03b2cc11d</t>
   </si>
   <si>
     <t>FILE_34</t>
@@ -626,16 +527,10 @@
     <t>SEQ_FILE_Q_R2.fastq.gz</t>
   </si>
   <si>
-    <t>060c20d2a467b08bf76b7b02db890ab731397d1bb3ddd951b38e72b12574cee5</t>
-  </si>
-  <si>
     <t>FILE_35</t>
   </si>
   <si>
     <t>SEQ_FILE_R_R1.fastq.gz</t>
-  </si>
-  <si>
-    <t>dc9ede6ab543d7d9ef796f074e912f589de847f62b9ec4742464110bf76a8e34</t>
   </si>
   <si>
     <t>FILE_36</t>
@@ -644,16 +539,10 @@
     <t>SEQ_FILE_R_R2.fastq.gz</t>
   </si>
   <si>
-    <t>2c04f666c91335b412dcf9b397d702edd2b26c7eda8b11547c7e76fb37752939</t>
-  </si>
-  <si>
     <t>FILE_37</t>
   </si>
   <si>
     <t>SEQ_FILE_S_R1.fastq.gz</t>
-  </si>
-  <si>
-    <t>e4c1abf47f7bd43bf7d341247392f27439aaa2b17d003a2aceb2b5b83bcd6d45</t>
   </si>
   <si>
     <t>FILE_38</t>
@@ -662,16 +551,10 @@
     <t>SEQ_FILE_S_R2.fastq.gz</t>
   </si>
   <si>
-    <t>83e3dfc7970238c7c3210dd4adaff223a1ccb4cdabbd19c91e217c02a31bd130</t>
-  </si>
-  <si>
     <t>FILE_39</t>
   </si>
   <si>
     <t>SEQ_FILE_T_R1.fastq.gz</t>
-  </si>
-  <si>
-    <t>d2206c38a47a85b8aec9b1be37f8c0e63a0d42689341e4b82ebce4dcd2195293</t>
   </si>
   <si>
     <t>FILE_40</t>
@@ -680,16 +563,10 @@
     <t>SEQ_FILE_T_R2.fastq.gz</t>
   </si>
   <si>
-    <t>07d5f9da9d4b50c419664fad70fb08773b1a81677adcc754bf04f43890d4c4fc</t>
-  </si>
-  <si>
     <t>FILE_41</t>
   </si>
   <si>
     <t>SEQ_FILE_U_R1.fastq.gz</t>
-  </si>
-  <si>
-    <t>65c50feed58a44b9bbe2f14185e0de2e5a9e0868fa25f4be4dd119a2e2b3fdaf</t>
   </si>
   <si>
     <t>FILE_42</t>
@@ -698,16 +575,10 @@
     <t>SEQ_FILE_U_R2.fastq.gz</t>
   </si>
   <si>
-    <t>1d6c077b6f5dbb8032858bdbd530c56b7ac6b1c4feb4be4a155ed456c4d01f1a</t>
-  </si>
-  <si>
     <t>FILE_43</t>
   </si>
   <si>
     <t>SEQ_FILE_V_R1.fastq.gz</t>
-  </si>
-  <si>
-    <t>236b00280ba6301fcc801473e2061ffa33215bc17579108ce99f197742959eb4</t>
   </si>
   <si>
     <t>DS_4</t>
@@ -719,16 +590,10 @@
     <t>SEQ_FILE_V_R2.fastq.gz</t>
   </si>
   <si>
-    <t>14888f079a8464a28370ff4aea9382cf94dd8155f77677b2c49deb8c249ce957</t>
-  </si>
-  <si>
     <t>FILE_45</t>
   </si>
   <si>
     <t>SEQ_FILE_W_R1.fastq.gz</t>
-  </si>
-  <si>
-    <t>cef8667aac74dd8cd057d087ffbddd3d1c8a653b6e595ce9a3cc567e013a0097</t>
   </si>
   <si>
     <t>FILE_46</t>
@@ -737,16 +602,10 @@
     <t>SEQ_FILE_W_R2.fastq.gz</t>
   </si>
   <si>
-    <t>333459bc3f4c12ca8f2f21d81d3883b15843e0e3b8497c213b1808693e927337</t>
-  </si>
-  <si>
     <t>FILE_47</t>
   </si>
   <si>
     <t>SEQ_FILE_X_R1.fastq.gz</t>
-  </si>
-  <si>
-    <t>2df56e140d380e0fedaf11a5a9789418250c2c1397c26b268f214ab9912d720c</t>
   </si>
   <si>
     <t>FILE_48</t>
@@ -755,16 +614,10 @@
     <t>SEQ_FILE_X_R2.fastq.gz</t>
   </si>
   <si>
-    <t>6951e467a10b198a699b7313e11a71cbc35eb968a9e98c2b6014f42b56120e1f</t>
-  </si>
-  <si>
     <t>FILE_49</t>
   </si>
   <si>
     <t>SEQ_FILE_Y_R1.fastq.gz</t>
-  </si>
-  <si>
-    <t>e50386fcd750c0e101a4910db71d2c825d0149e0b41ff701405191c514e493c5</t>
   </si>
   <si>
     <t>FILE_50</t>
@@ -773,25 +626,16 @@
     <t>SEQ_FILE_Y_R2.fastq.gz</t>
   </si>
   <si>
-    <t>80c54f88047174aed9f0354fefc8a8ba4cec2c0422eb03c627e902db7af7c70d</t>
-  </si>
-  <si>
     <t>FILE_51</t>
   </si>
   <si>
     <t>SEQ_FILE_Z_R1.fastq.gz</t>
   </si>
   <si>
-    <t>21bba04d8308dd3a46acd4da5aa67f14e13358fc8a3f84aa12b23a50d426dc7a</t>
-  </si>
-  <si>
     <t>FILE_52</t>
   </si>
   <si>
     <t>SEQ_FILE_Z_R2.fastq.gz</t>
-  </si>
-  <si>
-    <t>63175ec704f31428a49b21464d64746259f809c9669531def763b396e3641da9</t>
   </si>
   <si>
     <t>FORWARD</t>
@@ -885,6 +729,162 @@
   </si>
   <si>
     <t>The DAC institute</t>
+  </si>
+  <si>
+    <t>6d893451b8ed4159c9c31693894fdf6bb4e37c40705b977f315e00d75190d71e</t>
+  </si>
+  <si>
+    <t>1c9579c11d7e9eda0fd83beeb0d113e1d83af53aeba6747e251ebffbba0857a1</t>
+  </si>
+  <si>
+    <t>ac789d32d84025fd4f19f061d96279b719aaa8a92e7524aae00ec4d4a4d4c7b2</t>
+  </si>
+  <si>
+    <t>3451a704880381ece932362770fdfba9500970e3b61eac7e276cf832a696f6bc</t>
+  </si>
+  <si>
+    <t>2b5b7e057b3f29f65b81ce90e4d1f345989e82f0225dd0b688e3f7d17e188a5e</t>
+  </si>
+  <si>
+    <t>569792074549bd74dd021502bb8b93de93b2a020bebc36d85cb6860bd16523fd</t>
+  </si>
+  <si>
+    <t>6372bfee698058d7768ca8e051bff9f336dd0c6f256fad2802b89125b24be858</t>
+  </si>
+  <si>
+    <t>e830c31e41e4f210071b695eeab0672102d7ce4842d8f71ca4ff556661e767a9</t>
+  </si>
+  <si>
+    <t>f755b270ad22758bee88580199bc1edd8e0b5a366e0a49afbfe332753c7c65ff</t>
+  </si>
+  <si>
+    <t>98d69b3859d2ee3a6c047e64d75ff26081d1e01cc283dcffe7982034b5786c7c</t>
+  </si>
+  <si>
+    <t>ca8b627793c09722a8a67df9a86ca992d9c611da67f9e09dd82fa5fbbdfc888f</t>
+  </si>
+  <si>
+    <t>74473a16db3d3f037921fcb637c709a859f435ebb92acc13026dae56e82ce871</t>
+  </si>
+  <si>
+    <t>87915df7c6c014a380f9fded427b0650d15094b93b396e36f026ed8604ef29c2</t>
+  </si>
+  <si>
+    <t>61ea1a00a870846b7eb5af23a7d1642a12e0ae89dc0d8184ce01bc86641ba9e1</t>
+  </si>
+  <si>
+    <t>421a7518062f8620a046175510c42c27425bd39ee527c69eabdfde5b8cca21a8</t>
+  </si>
+  <si>
+    <t>31be4a412b08df968bfab48754cc87cc14a71c4a241110ad881eeee2e692c560</t>
+  </si>
+  <si>
+    <t>1aea8f7a679c57e09560176bd21e4b0c113f1975b8fe6452e312e23b780e7e04</t>
+  </si>
+  <si>
+    <t>acd38db5f1dd66f5360f09cf0b75917f840dd0cfae7c55de0ab5e78d254928ab</t>
+  </si>
+  <si>
+    <t>92a779a9456e487bcb6f64c37fe273d0d1e8ce63eaa04bffb1fe34e8f9ab1ca3</t>
+  </si>
+  <si>
+    <t>21168bff3d6d6427774100d1ebac454596d13e9ba8f9e532582ad61115d8dfb6</t>
+  </si>
+  <si>
+    <t>cbddfe7c8cc7d86036a9a89427b923b420618947c5b7e52cfad4f10637285d10</t>
+  </si>
+  <si>
+    <t>1adf6fe8f39577ba9ee04ecd54f7993171a38c4adf29af9e80479125dc125c7d</t>
+  </si>
+  <si>
+    <t>868f79790567d12c788da81e06fad6660dea7005a29d22113ece988cae6e3789</t>
+  </si>
+  <si>
+    <t>0aa199655fbcfd3210c6b1b6e448a5e6f550fab757020d00afab9da98d299f38</t>
+  </si>
+  <si>
+    <t>387528dc9007900d4c325d5f30c698b4e245cdceaafd6ede749e888f2c2d8b01</t>
+  </si>
+  <si>
+    <t>a5a665c7c9ac7869feefa638bc0c36c1277bf3806a5ca0dab6612a231b110c47</t>
+  </si>
+  <si>
+    <t>ff3407f770f6d8e3fd6deb58bea3812ebe7dc72a23530f83a9dc8b874b15678c</t>
+  </si>
+  <si>
+    <t>3bae81b1158274db6eb98914c45d35fa36dcd8a82436605fd036a371abf95d19</t>
+  </si>
+  <si>
+    <t>6d816fbfca7b79ce737b9ae2fc72ffb06b74fbcbf5fd1a572104eae2b1f87eea</t>
+  </si>
+  <si>
+    <t>c92b678b296e13393d96755fc4130bf567cb0ec76fc0c830cd5010c91fccf896</t>
+  </si>
+  <si>
+    <t>c464ca6e3fddb03069685ee61a16c02de708e114f5ed8c705c7c6feb974bdbcd</t>
+  </si>
+  <si>
+    <t>8cb0040d4e84f4f2c4f27a48d41864eb49f69719c2bb7e012e54cbf62d273692</t>
+  </si>
+  <si>
+    <t>9dea3f529fe2bf63657563630e9933a8883898ae449dd002b5eadf0031976909</t>
+  </si>
+  <si>
+    <t>6efad42ae46e2d2f9298ba8d206ae9490556b4ab204cf205106f5a6a5104c961</t>
+  </si>
+  <si>
+    <t>17e1149486c22e92abae2ff6534d9e2e0657f528aa96e0ecf24ab0164f484000</t>
+  </si>
+  <si>
+    <t>14e5353efad785d079a84e667398c4e47dca7769de5a8b4824b93039c02cc386</t>
+  </si>
+  <si>
+    <t>a3955d3579dfdb98c78d7eadab1045f2af24c311a679969d48944c5a7360d6c2</t>
+  </si>
+  <si>
+    <t>1cbec623ac2eec0e460433ce1b9d7dfe82f704a61ed2154d091865a38cb7f396</t>
+  </si>
+  <si>
+    <t>4024ee97fc733989e1f45a70c3afcbe14361f620a57af4f02c3e5f76befc2380</t>
+  </si>
+  <si>
+    <t>25b3ab9f971a12defb584e56f4e9bbe360c888f6025fc8b0fcbcf0075b522311</t>
+  </si>
+  <si>
+    <t>97d7d476e24a2d824259eda9877e22e8a40acd80b89e1f40cfd82567d9bc0fb5</t>
+  </si>
+  <si>
+    <t>a9e3af6a3f682dbf7aa672b46d293ae64da87829e7583d88e158c662b01c5e8d</t>
+  </si>
+  <si>
+    <t>f02e10ccabd47e0d1408d1b730b86f033b803ab7a8a3b244eaad8b190365decd</t>
+  </si>
+  <si>
+    <t>e09a51143ae290f7a914e36a045ce0cc1d9c388ea32bc2e33ba69cece7b069a7</t>
+  </si>
+  <si>
+    <t>07ce01d6f7b8d142e2b686fac6afce142ca969c763de623eedbfdbb72745746d</t>
+  </si>
+  <si>
+    <t>ad9938d9a42e0ae81035842ba7450026b9aa81299ce5fa733cdbd3597b47c317</t>
+  </si>
+  <si>
+    <t>7ac08879fca2f038419db2cd1617a124051a1da42a67875cda64b8a6c9b84c9a</t>
+  </si>
+  <si>
+    <t>f07649e2d937b32157f739f0d59dfc930336fb101f2004495a7827c1bd538409</t>
+  </si>
+  <si>
+    <t>cbd192a0bfc7deec6a1f7abadbea391eda38d1002f0b90e1dfb71dc4c965e647</t>
+  </si>
+  <si>
+    <t>9fa04196439164392c80761d8be02b6b3b5a573249fc0fcda42a795feb8e93f3</t>
+  </si>
+  <si>
+    <t>77d450e1497715383931c16df4180e8cc266678b30969884967cb938231cedc6</t>
+  </si>
+  <si>
+    <t>ba293f21da806db924a4d906641355dd6f6bb753dabbadd990fac7ec54150ceb</t>
   </si>
 </sst>
 </file>
@@ -9524,7 +9524,9 @@
   </sheetPr>
   <dimension ref="A1:I1006"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -9721,1498 +9723,1498 @@
         <v>91</v>
       </c>
       <c r="E7" s="6">
-        <v>92161</v>
+        <v>2049</v>
       </c>
       <c r="F7" s="6" t="s">
+        <v>230</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>199</v>
+      </c>
+      <c r="H7" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="G7" s="6" t="s">
-        <v>251</v>
-      </c>
-      <c r="H7" s="6" t="s">
+      <c r="I7" s="6" t="s">
         <v>93</v>
-      </c>
-      <c r="I7" s="6" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>87</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D8" s="6" t="s">
         <v>91</v>
       </c>
       <c r="E8" s="6">
-        <v>92161</v>
+        <v>6145</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>97</v>
+        <v>231</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>252</v>
+        <v>200</v>
       </c>
       <c r="H8" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="I8" s="6" t="s">
         <v>93</v>
-      </c>
-      <c r="I8" s="6" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>87</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>91</v>
       </c>
       <c r="E9" s="6">
-        <v>92161</v>
+        <v>4097</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>100</v>
+        <v>232</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>251</v>
+        <v>199</v>
       </c>
       <c r="H9" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="I9" s="6" t="s">
         <v>93</v>
-      </c>
-      <c r="I9" s="6" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>87</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="D10" s="6" t="s">
         <v>91</v>
       </c>
       <c r="E10" s="6">
-        <v>92161</v>
+        <v>6145</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>103</v>
+        <v>233</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>252</v>
+        <v>200</v>
       </c>
       <c r="H10" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="I10" s="6" t="s">
         <v>93</v>
-      </c>
-      <c r="I10" s="6" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>87</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="D11" s="6" t="s">
         <v>91</v>
       </c>
       <c r="E11" s="6">
-        <v>92161</v>
+        <v>6145</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>106</v>
+        <v>234</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>251</v>
+        <v>199</v>
       </c>
       <c r="H11" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="I11" s="6" t="s">
         <v>93</v>
-      </c>
-      <c r="I11" s="6" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>87</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="D12" s="6" t="s">
         <v>91</v>
       </c>
       <c r="E12" s="6">
-        <v>92161</v>
+        <v>8193</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>109</v>
+        <v>235</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>252</v>
+        <v>200</v>
       </c>
       <c r="H12" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="I12" s="6" t="s">
         <v>93</v>
-      </c>
-      <c r="I12" s="6" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>87</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="D13" s="6" t="s">
         <v>91</v>
       </c>
       <c r="E13" s="6">
-        <v>92161</v>
+        <v>4097</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>112</v>
+        <v>236</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>251</v>
+        <v>199</v>
       </c>
       <c r="H13" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="I13" s="6" t="s">
         <v>93</v>
-      </c>
-      <c r="I13" s="6" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="B14" s="6" t="s">
         <v>87</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="D14" s="6" t="s">
         <v>91</v>
       </c>
       <c r="E14" s="6">
-        <v>92161</v>
+        <v>4097</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>115</v>
+        <v>237</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>252</v>
+        <v>200</v>
       </c>
       <c r="H14" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="I14" s="6" t="s">
         <v>93</v>
-      </c>
-      <c r="I14" s="6" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="B15" s="6" t="s">
         <v>87</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="D15" s="6" t="s">
         <v>91</v>
       </c>
       <c r="E15" s="6">
-        <v>92161</v>
+        <v>2049</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>118</v>
+        <v>238</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>251</v>
+        <v>199</v>
       </c>
       <c r="H15" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="I15" s="6" t="s">
         <v>93</v>
-      </c>
-      <c r="I15" s="6" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="B16" s="6" t="s">
         <v>87</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="D16" s="6" t="s">
         <v>91</v>
       </c>
       <c r="E16" s="6">
-        <v>92161</v>
+        <v>8193</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>121</v>
+        <v>239</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>252</v>
+        <v>200</v>
       </c>
       <c r="H16" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="I16" s="6" t="s">
         <v>93</v>
-      </c>
-      <c r="I16" s="6" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="B17" s="6" t="s">
         <v>87</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>123</v>
+        <v>113</v>
       </c>
       <c r="D17" s="6" t="s">
         <v>91</v>
       </c>
       <c r="E17" s="6">
-        <v>92161</v>
+        <v>6145</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>124</v>
+        <v>240</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>251</v>
+        <v>199</v>
       </c>
       <c r="H17" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="I17" s="6" t="s">
         <v>93</v>
-      </c>
-      <c r="I17" s="6" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="s">
-        <v>125</v>
+        <v>114</v>
       </c>
       <c r="B18" s="6" t="s">
         <v>87</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>126</v>
+        <v>115</v>
       </c>
       <c r="D18" s="6" t="s">
         <v>91</v>
       </c>
       <c r="E18" s="6">
-        <v>92161</v>
+        <v>8193</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>127</v>
+        <v>241</v>
       </c>
       <c r="G18" s="6" t="s">
-        <v>252</v>
+        <v>200</v>
       </c>
       <c r="H18" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="I18" s="6" t="s">
         <v>93</v>
-      </c>
-      <c r="I18" s="6" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" s="6" t="s">
-        <v>128</v>
+        <v>116</v>
       </c>
       <c r="B19" s="6" t="s">
         <v>87</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>129</v>
+        <v>117</v>
       </c>
       <c r="D19" s="6" t="s">
         <v>91</v>
       </c>
       <c r="E19" s="6">
-        <v>92161</v>
+        <v>2049</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>130</v>
+        <v>242</v>
       </c>
       <c r="G19" s="6" t="s">
-        <v>251</v>
+        <v>199</v>
       </c>
       <c r="H19" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="I19" s="6" t="s">
         <v>93</v>
-      </c>
-      <c r="I19" s="6" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="6" t="s">
-        <v>131</v>
+        <v>118</v>
       </c>
       <c r="B20" s="6" t="s">
         <v>87</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>132</v>
+        <v>119</v>
       </c>
       <c r="D20" s="6" t="s">
         <v>91</v>
       </c>
       <c r="E20" s="6">
-        <v>92161</v>
+        <v>4097</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>133</v>
+        <v>243</v>
       </c>
       <c r="G20" s="6" t="s">
-        <v>252</v>
+        <v>200</v>
       </c>
       <c r="H20" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="I20" s="6" t="s">
         <v>93</v>
-      </c>
-      <c r="I20" s="6" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="6" t="s">
-        <v>134</v>
+        <v>120</v>
       </c>
       <c r="B21" s="6" t="s">
         <v>87</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>135</v>
+        <v>121</v>
       </c>
       <c r="D21" s="6" t="s">
         <v>91</v>
       </c>
       <c r="E21" s="6">
-        <v>92161</v>
+        <v>4097</v>
       </c>
       <c r="F21" s="6" t="s">
-        <v>136</v>
+        <v>244</v>
       </c>
       <c r="G21" s="6" t="s">
-        <v>251</v>
+        <v>199</v>
       </c>
       <c r="H21" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="I21" s="6" t="s">
         <v>93</v>
-      </c>
-      <c r="I21" s="6" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="6" t="s">
-        <v>137</v>
+        <v>122</v>
       </c>
       <c r="B22" s="6" t="s">
         <v>87</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>138</v>
+        <v>123</v>
       </c>
       <c r="D22" s="6" t="s">
         <v>91</v>
       </c>
       <c r="E22" s="6">
-        <v>92161</v>
+        <v>2049</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>139</v>
+        <v>245</v>
       </c>
       <c r="G22" s="6" t="s">
-        <v>252</v>
+        <v>200</v>
       </c>
       <c r="H22" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="I22" s="6" t="s">
         <v>93</v>
-      </c>
-      <c r="I22" s="6" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="6" t="s">
-        <v>140</v>
+        <v>124</v>
       </c>
       <c r="B23" s="6" t="s">
         <v>87</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>141</v>
+        <v>125</v>
       </c>
       <c r="D23" s="6" t="s">
         <v>91</v>
       </c>
       <c r="E23" s="6">
-        <v>92161</v>
+        <v>6145</v>
       </c>
       <c r="F23" s="6" t="s">
-        <v>142</v>
+        <v>246</v>
       </c>
       <c r="G23" s="6" t="s">
-        <v>251</v>
+        <v>199</v>
       </c>
       <c r="H23" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I23" s="6" t="s">
-        <v>143</v>
+        <v>126</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="6" t="s">
-        <v>144</v>
+        <v>127</v>
       </c>
       <c r="B24" s="6" t="s">
         <v>87</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>145</v>
+        <v>128</v>
       </c>
       <c r="D24" s="6" t="s">
         <v>91</v>
       </c>
       <c r="E24" s="6">
-        <v>92161</v>
+        <v>4097</v>
       </c>
       <c r="F24" s="6" t="s">
-        <v>146</v>
+        <v>247</v>
       </c>
       <c r="G24" s="6" t="s">
-        <v>252</v>
+        <v>200</v>
       </c>
       <c r="H24" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I24" s="6" t="s">
-        <v>143</v>
+        <v>126</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="6" t="s">
-        <v>147</v>
+        <v>129</v>
       </c>
       <c r="B25" s="6" t="s">
         <v>87</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>148</v>
+        <v>130</v>
       </c>
       <c r="D25" s="6" t="s">
         <v>91</v>
       </c>
       <c r="E25" s="6">
-        <v>92161</v>
+        <v>6145</v>
       </c>
       <c r="F25" s="6" t="s">
-        <v>149</v>
+        <v>248</v>
       </c>
       <c r="G25" s="6" t="s">
-        <v>251</v>
+        <v>199</v>
       </c>
       <c r="H25" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I25" s="6" t="s">
-        <v>143</v>
+        <v>126</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="6" t="s">
-        <v>150</v>
+        <v>131</v>
       </c>
       <c r="B26" s="6" t="s">
         <v>87</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>151</v>
+        <v>132</v>
       </c>
       <c r="D26" s="6" t="s">
         <v>91</v>
       </c>
       <c r="E26" s="6">
-        <v>92161</v>
+        <v>8193</v>
       </c>
       <c r="F26" s="6" t="s">
-        <v>152</v>
+        <v>249</v>
       </c>
       <c r="G26" s="6" t="s">
-        <v>252</v>
+        <v>200</v>
       </c>
       <c r="H26" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I26" s="6" t="s">
-        <v>143</v>
+        <v>126</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="6" t="s">
-        <v>153</v>
+        <v>133</v>
       </c>
       <c r="B27" s="6" t="s">
         <v>87</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>154</v>
+        <v>134</v>
       </c>
       <c r="D27" s="6" t="s">
         <v>91</v>
       </c>
       <c r="E27" s="6">
-        <v>92161</v>
+        <v>6145</v>
       </c>
       <c r="F27" s="6" t="s">
-        <v>155</v>
+        <v>250</v>
       </c>
       <c r="G27" s="6" t="s">
-        <v>251</v>
+        <v>199</v>
       </c>
       <c r="H27" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I27" s="6" t="s">
-        <v>143</v>
+        <v>126</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="6" t="s">
-        <v>156</v>
+        <v>135</v>
       </c>
       <c r="B28" s="6" t="s">
         <v>87</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>157</v>
+        <v>136</v>
       </c>
       <c r="D28" s="6" t="s">
         <v>91</v>
       </c>
       <c r="E28" s="6">
-        <v>92161</v>
+        <v>8193</v>
       </c>
       <c r="F28" s="6" t="s">
-        <v>158</v>
+        <v>251</v>
       </c>
       <c r="G28" s="6" t="s">
-        <v>252</v>
+        <v>200</v>
       </c>
       <c r="H28" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I28" s="6" t="s">
-        <v>143</v>
+        <v>126</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" s="6" t="s">
-        <v>159</v>
+        <v>137</v>
       </c>
       <c r="B29" s="6" t="s">
         <v>87</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>160</v>
+        <v>138</v>
       </c>
       <c r="D29" s="6" t="s">
         <v>91</v>
       </c>
       <c r="E29" s="6">
-        <v>92161</v>
+        <v>4097</v>
       </c>
       <c r="F29" s="6" t="s">
-        <v>161</v>
+        <v>252</v>
       </c>
       <c r="G29" s="6" t="s">
-        <v>251</v>
+        <v>199</v>
       </c>
       <c r="H29" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I29" s="6" t="s">
-        <v>162</v>
+        <v>139</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" s="6" t="s">
-        <v>163</v>
+        <v>140</v>
       </c>
       <c r="B30" s="6" t="s">
         <v>87</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>164</v>
+        <v>141</v>
       </c>
       <c r="D30" s="6" t="s">
         <v>91</v>
       </c>
       <c r="E30" s="6">
-        <v>92161</v>
+        <v>8193</v>
       </c>
       <c r="F30" s="6" t="s">
-        <v>165</v>
+        <v>253</v>
       </c>
       <c r="G30" s="6" t="s">
-        <v>252</v>
+        <v>200</v>
       </c>
       <c r="H30" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I30" s="6" t="s">
-        <v>162</v>
+        <v>139</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A31" s="6" t="s">
-        <v>166</v>
+        <v>142</v>
       </c>
       <c r="B31" s="6" t="s">
         <v>88</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>167</v>
+        <v>143</v>
       </c>
       <c r="D31" s="6" t="s">
         <v>91</v>
       </c>
       <c r="E31" s="6">
-        <v>92161</v>
+        <v>8193</v>
       </c>
       <c r="F31" s="6" t="s">
-        <v>168</v>
+        <v>254</v>
       </c>
       <c r="G31" s="6" t="s">
-        <v>251</v>
+        <v>199</v>
       </c>
       <c r="H31" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I31" s="6" t="s">
-        <v>162</v>
+        <v>139</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A32" s="6" t="s">
-        <v>169</v>
+        <v>144</v>
       </c>
       <c r="B32" s="6" t="s">
         <v>88</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>170</v>
+        <v>145</v>
       </c>
       <c r="D32" s="6" t="s">
         <v>91</v>
       </c>
       <c r="E32" s="6">
-        <v>92161</v>
+        <v>8193</v>
       </c>
       <c r="F32" s="6" t="s">
-        <v>171</v>
+        <v>255</v>
       </c>
       <c r="G32" s="6" t="s">
-        <v>252</v>
+        <v>200</v>
       </c>
       <c r="H32" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I32" s="6" t="s">
-        <v>162</v>
+        <v>139</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A33" s="6" t="s">
-        <v>172</v>
+        <v>146</v>
       </c>
       <c r="B33" s="6" t="s">
         <v>88</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>173</v>
+        <v>147</v>
       </c>
       <c r="D33" s="6" t="s">
         <v>91</v>
       </c>
       <c r="E33" s="6">
-        <v>92161</v>
+        <v>4097</v>
       </c>
       <c r="F33" s="6" t="s">
-        <v>174</v>
+        <v>256</v>
       </c>
       <c r="G33" s="6" t="s">
-        <v>251</v>
+        <v>199</v>
       </c>
       <c r="H33" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I33" s="6" t="s">
-        <v>162</v>
+        <v>139</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A34" s="6" t="s">
-        <v>175</v>
+        <v>148</v>
       </c>
       <c r="B34" s="6" t="s">
         <v>88</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>176</v>
+        <v>149</v>
       </c>
       <c r="D34" s="6" t="s">
         <v>91</v>
       </c>
       <c r="E34" s="6">
-        <v>92161</v>
+        <v>4097</v>
       </c>
       <c r="F34" s="6" t="s">
-        <v>177</v>
+        <v>257</v>
       </c>
       <c r="G34" s="6" t="s">
-        <v>252</v>
+        <v>200</v>
       </c>
       <c r="H34" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I34" s="6" t="s">
-        <v>162</v>
+        <v>139</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A35" s="6" t="s">
-        <v>178</v>
+        <v>150</v>
       </c>
       <c r="B35" s="6" t="s">
         <v>88</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>179</v>
+        <v>151</v>
       </c>
       <c r="D35" s="6" t="s">
         <v>91</v>
       </c>
       <c r="E35" s="6">
-        <v>92161</v>
+        <v>2049</v>
       </c>
       <c r="F35" s="6" t="s">
-        <v>180</v>
+        <v>258</v>
       </c>
       <c r="G35" s="6" t="s">
-        <v>251</v>
+        <v>199</v>
       </c>
       <c r="H35" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I35" s="6" t="s">
-        <v>162</v>
+        <v>139</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A36" s="6" t="s">
-        <v>181</v>
+        <v>152</v>
       </c>
       <c r="B36" s="6" t="s">
         <v>88</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>182</v>
+        <v>153</v>
       </c>
       <c r="D36" s="6" t="s">
         <v>91</v>
       </c>
       <c r="E36" s="6">
-        <v>92161</v>
+        <v>6145</v>
       </c>
       <c r="F36" s="6" t="s">
-        <v>183</v>
+        <v>259</v>
       </c>
       <c r="G36" s="6" t="s">
-        <v>252</v>
+        <v>200</v>
       </c>
       <c r="H36" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I36" s="6" t="s">
-        <v>162</v>
+        <v>139</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A37" s="6" t="s">
-        <v>184</v>
+        <v>154</v>
       </c>
       <c r="B37" s="6" t="s">
         <v>88</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>185</v>
+        <v>155</v>
       </c>
       <c r="D37" s="6" t="s">
         <v>91</v>
       </c>
       <c r="E37" s="6">
-        <v>92161</v>
+        <v>6145</v>
       </c>
       <c r="F37" s="6" t="s">
-        <v>186</v>
+        <v>260</v>
       </c>
       <c r="G37" s="6" t="s">
-        <v>251</v>
+        <v>199</v>
       </c>
       <c r="H37" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I37" s="6" t="s">
-        <v>162</v>
+        <v>139</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A38" s="6" t="s">
-        <v>187</v>
+        <v>156</v>
       </c>
       <c r="B38" s="6" t="s">
         <v>88</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>188</v>
+        <v>157</v>
       </c>
       <c r="D38" s="6" t="s">
         <v>91</v>
       </c>
       <c r="E38" s="6">
-        <v>92161</v>
+        <v>2049</v>
       </c>
       <c r="F38" s="6" t="s">
-        <v>189</v>
+        <v>261</v>
       </c>
       <c r="G38" s="6" t="s">
-        <v>252</v>
+        <v>200</v>
       </c>
       <c r="H38" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I38" s="6" t="s">
-        <v>162</v>
+        <v>139</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A39" s="6" t="s">
-        <v>190</v>
+        <v>158</v>
       </c>
       <c r="B39" s="6" t="s">
         <v>88</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>191</v>
+        <v>159</v>
       </c>
       <c r="D39" s="6" t="s">
         <v>91</v>
       </c>
       <c r="E39" s="6">
-        <v>92161</v>
+        <v>8193</v>
       </c>
       <c r="F39" s="6" t="s">
-        <v>192</v>
+        <v>262</v>
       </c>
       <c r="G39" s="6" t="s">
-        <v>251</v>
+        <v>199</v>
       </c>
       <c r="H39" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I39" s="6" t="s">
-        <v>162</v>
+        <v>139</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A40" s="6" t="s">
-        <v>193</v>
+        <v>160</v>
       </c>
       <c r="B40" s="6" t="s">
         <v>88</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>194</v>
+        <v>161</v>
       </c>
       <c r="D40" s="6" t="s">
         <v>91</v>
       </c>
       <c r="E40" s="6">
-        <v>92161</v>
+        <v>8193</v>
       </c>
       <c r="F40" s="6" t="s">
-        <v>195</v>
+        <v>263</v>
       </c>
       <c r="G40" s="6" t="s">
-        <v>252</v>
+        <v>200</v>
       </c>
       <c r="H40" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I40" s="6" t="s">
-        <v>162</v>
+        <v>139</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" s="6" t="s">
-        <v>196</v>
+        <v>162</v>
       </c>
       <c r="B41" s="6" t="s">
         <v>88</v>
       </c>
       <c r="C41" s="6" t="s">
-        <v>197</v>
+        <v>163</v>
       </c>
       <c r="D41" s="6" t="s">
         <v>91</v>
       </c>
       <c r="E41" s="6">
-        <v>92161</v>
-      </c>
-      <c r="F41" s="6" t="s">
-        <v>198</v>
+        <v>8193</v>
+      </c>
+      <c r="F41" s="16" t="s">
+        <v>264</v>
       </c>
       <c r="G41" s="6" t="s">
-        <v>251</v>
+        <v>199</v>
       </c>
       <c r="H41" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I41" s="6" t="s">
-        <v>162</v>
+        <v>139</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A42" s="6" t="s">
-        <v>199</v>
+        <v>164</v>
       </c>
       <c r="B42" s="6" t="s">
         <v>88</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>200</v>
+        <v>165</v>
       </c>
       <c r="D42" s="6" t="s">
         <v>91</v>
       </c>
       <c r="E42" s="6">
-        <v>92161</v>
-      </c>
-      <c r="F42" s="6" t="s">
-        <v>201</v>
+        <v>6145</v>
+      </c>
+      <c r="F42" s="16" t="s">
+        <v>265</v>
       </c>
       <c r="G42" s="6" t="s">
-        <v>252</v>
+        <v>200</v>
       </c>
       <c r="H42" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I42" s="6" t="s">
-        <v>162</v>
+        <v>139</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A43" s="6" t="s">
-        <v>202</v>
+        <v>166</v>
       </c>
       <c r="B43" s="6" t="s">
         <v>88</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>203</v>
+        <v>167</v>
       </c>
       <c r="D43" s="6" t="s">
         <v>91</v>
       </c>
       <c r="E43" s="6">
-        <v>92161</v>
+        <v>4097</v>
       </c>
       <c r="F43" s="6" t="s">
-        <v>204</v>
+        <v>266</v>
       </c>
       <c r="G43" s="6" t="s">
-        <v>251</v>
+        <v>199</v>
       </c>
       <c r="H43" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I43" s="6" t="s">
-        <v>162</v>
+        <v>139</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A44" s="6" t="s">
-        <v>205</v>
+        <v>168</v>
       </c>
       <c r="B44" s="6" t="s">
         <v>88</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>206</v>
+        <v>169</v>
       </c>
       <c r="D44" s="6" t="s">
         <v>91</v>
       </c>
       <c r="E44" s="6">
-        <v>92161</v>
+        <v>2049</v>
       </c>
       <c r="F44" s="6" t="s">
-        <v>207</v>
+        <v>267</v>
       </c>
       <c r="G44" s="6" t="s">
-        <v>252</v>
+        <v>200</v>
       </c>
       <c r="H44" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I44" s="6" t="s">
-        <v>162</v>
+        <v>139</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A45" s="6" t="s">
-        <v>208</v>
+        <v>170</v>
       </c>
       <c r="B45" s="6" t="s">
         <v>88</v>
       </c>
       <c r="C45" s="6" t="s">
-        <v>209</v>
+        <v>171</v>
       </c>
       <c r="D45" s="6" t="s">
         <v>91</v>
       </c>
       <c r="E45" s="6">
-        <v>92161</v>
+        <v>6145</v>
       </c>
       <c r="F45" s="6" t="s">
-        <v>210</v>
+        <v>268</v>
       </c>
       <c r="G45" s="6" t="s">
-        <v>251</v>
+        <v>199</v>
       </c>
       <c r="H45" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I45" s="6" t="s">
-        <v>162</v>
+        <v>139</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A46" s="6" t="s">
-        <v>211</v>
+        <v>172</v>
       </c>
       <c r="B46" s="6" t="s">
         <v>88</v>
       </c>
       <c r="C46" s="6" t="s">
-        <v>212</v>
+        <v>173</v>
       </c>
       <c r="D46" s="6" t="s">
         <v>91</v>
       </c>
       <c r="E46" s="6">
-        <v>92161</v>
+        <v>8193</v>
       </c>
       <c r="F46" s="6" t="s">
-        <v>213</v>
+        <v>269</v>
       </c>
       <c r="G46" s="6" t="s">
-        <v>252</v>
+        <v>200</v>
       </c>
       <c r="H46" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I46" s="6" t="s">
-        <v>162</v>
+        <v>139</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A47" s="6" t="s">
-        <v>214</v>
+        <v>174</v>
       </c>
       <c r="B47" s="6" t="s">
         <v>88</v>
       </c>
       <c r="C47" s="6" t="s">
-        <v>215</v>
+        <v>175</v>
       </c>
       <c r="D47" s="6" t="s">
         <v>91</v>
       </c>
       <c r="E47" s="6">
-        <v>92161</v>
+        <v>4097</v>
       </c>
       <c r="F47" s="6" t="s">
-        <v>216</v>
+        <v>270</v>
       </c>
       <c r="G47" s="6" t="s">
-        <v>251</v>
+        <v>199</v>
       </c>
       <c r="H47" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I47" s="6" t="s">
-        <v>162</v>
+        <v>139</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A48" s="6" t="s">
-        <v>217</v>
+        <v>176</v>
       </c>
       <c r="B48" s="6" t="s">
         <v>88</v>
       </c>
       <c r="C48" s="6" t="s">
-        <v>218</v>
+        <v>177</v>
       </c>
       <c r="D48" s="6" t="s">
         <v>91</v>
       </c>
       <c r="E48" s="6">
-        <v>92161</v>
+        <v>6145</v>
       </c>
       <c r="F48" s="6" t="s">
-        <v>219</v>
+        <v>271</v>
       </c>
       <c r="G48" s="6" t="s">
-        <v>252</v>
+        <v>200</v>
       </c>
       <c r="H48" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I48" s="6" t="s">
-        <v>162</v>
+        <v>139</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A49" s="6" t="s">
-        <v>220</v>
+        <v>178</v>
       </c>
       <c r="B49" s="6" t="s">
         <v>88</v>
       </c>
       <c r="C49" s="6" t="s">
-        <v>221</v>
+        <v>179</v>
       </c>
       <c r="D49" s="6" t="s">
         <v>91</v>
       </c>
       <c r="E49" s="6">
-        <v>92161</v>
+        <v>8193</v>
       </c>
       <c r="F49" s="6" t="s">
-        <v>222</v>
+        <v>272</v>
       </c>
       <c r="G49" s="6" t="s">
-        <v>251</v>
+        <v>199</v>
       </c>
       <c r="H49" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I49" s="6" t="s">
-        <v>223</v>
+        <v>180</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A50" s="6" t="s">
-        <v>224</v>
+        <v>181</v>
       </c>
       <c r="B50" s="6" t="s">
         <v>88</v>
       </c>
       <c r="C50" s="6" t="s">
-        <v>225</v>
+        <v>182</v>
       </c>
       <c r="D50" s="6" t="s">
         <v>91</v>
       </c>
       <c r="E50" s="6">
-        <v>92161</v>
+        <v>4097</v>
       </c>
       <c r="F50" s="6" t="s">
-        <v>226</v>
+        <v>273</v>
       </c>
       <c r="G50" s="6" t="s">
-        <v>252</v>
+        <v>200</v>
       </c>
       <c r="H50" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I50" s="6" t="s">
-        <v>223</v>
+        <v>180</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A51" s="6" t="s">
-        <v>227</v>
+        <v>183</v>
       </c>
       <c r="B51" s="6" t="s">
         <v>88</v>
       </c>
       <c r="C51" s="6" t="s">
-        <v>228</v>
+        <v>184</v>
       </c>
       <c r="D51" s="6" t="s">
         <v>91</v>
       </c>
       <c r="E51" s="6">
-        <v>92161</v>
+        <v>8193</v>
       </c>
       <c r="F51" s="6" t="s">
-        <v>229</v>
+        <v>274</v>
       </c>
       <c r="G51" s="6" t="s">
-        <v>251</v>
+        <v>199</v>
       </c>
       <c r="H51" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I51" s="6" t="s">
-        <v>223</v>
+        <v>180</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A52" s="6" t="s">
-        <v>230</v>
+        <v>185</v>
       </c>
       <c r="B52" s="6" t="s">
         <v>88</v>
       </c>
       <c r="C52" s="6" t="s">
-        <v>231</v>
+        <v>186</v>
       </c>
       <c r="D52" s="6" t="s">
         <v>91</v>
       </c>
       <c r="E52" s="6">
-        <v>92161</v>
+        <v>6145</v>
       </c>
       <c r="F52" s="6" t="s">
-        <v>232</v>
+        <v>275</v>
       </c>
       <c r="G52" s="6" t="s">
-        <v>252</v>
+        <v>200</v>
       </c>
       <c r="H52" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I52" s="6" t="s">
-        <v>223</v>
+        <v>180</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A53" s="6" t="s">
-        <v>233</v>
+        <v>187</v>
       </c>
       <c r="B53" s="6" t="s">
         <v>88</v>
       </c>
       <c r="C53" s="6" t="s">
-        <v>234</v>
+        <v>188</v>
       </c>
       <c r="D53" s="6" t="s">
         <v>91</v>
       </c>
       <c r="E53" s="6">
-        <v>92161</v>
+        <v>6145</v>
       </c>
       <c r="F53" s="6" t="s">
-        <v>235</v>
+        <v>276</v>
       </c>
       <c r="G53" s="6" t="s">
-        <v>251</v>
+        <v>199</v>
       </c>
       <c r="H53" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I53" s="6" t="s">
-        <v>223</v>
+        <v>180</v>
       </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A54" s="6" t="s">
-        <v>236</v>
+        <v>189</v>
       </c>
       <c r="B54" s="6" t="s">
         <v>88</v>
       </c>
       <c r="C54" s="6" t="s">
-        <v>237</v>
+        <v>190</v>
       </c>
       <c r="D54" s="6" t="s">
         <v>91</v>
       </c>
       <c r="E54" s="6">
-        <v>92161</v>
+        <v>8193</v>
       </c>
       <c r="F54" s="16" t="s">
-        <v>238</v>
+        <v>277</v>
       </c>
       <c r="G54" s="6" t="s">
-        <v>252</v>
+        <v>200</v>
       </c>
       <c r="H54" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I54" s="6" t="s">
-        <v>223</v>
+        <v>180</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A55" s="6" t="s">
-        <v>239</v>
+        <v>191</v>
       </c>
       <c r="B55" s="6" t="s">
         <v>88</v>
       </c>
       <c r="C55" s="6" t="s">
-        <v>240</v>
+        <v>192</v>
       </c>
       <c r="D55" s="6" t="s">
         <v>91</v>
       </c>
       <c r="E55" s="6">
-        <v>92161</v>
+        <v>4097</v>
       </c>
       <c r="F55" s="6" t="s">
-        <v>241</v>
+        <v>278</v>
       </c>
       <c r="G55" s="6" t="s">
-        <v>251</v>
+        <v>199</v>
       </c>
       <c r="H55" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I55" s="6" t="s">
-        <v>223</v>
+        <v>180</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A56" s="6" t="s">
-        <v>242</v>
+        <v>193</v>
       </c>
       <c r="B56" s="6" t="s">
         <v>88</v>
       </c>
       <c r="C56" s="6" t="s">
-        <v>243</v>
+        <v>194</v>
       </c>
       <c r="D56" s="6" t="s">
         <v>91</v>
       </c>
       <c r="E56" s="6">
-        <v>92161</v>
+        <v>4097</v>
       </c>
       <c r="F56" s="6" t="s">
-        <v>244</v>
+        <v>279</v>
       </c>
       <c r="G56" s="6" t="s">
-        <v>252</v>
+        <v>200</v>
       </c>
       <c r="H56" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I56" s="6" t="s">
-        <v>223</v>
+        <v>180</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A57" s="6" t="s">
-        <v>245</v>
+        <v>195</v>
       </c>
       <c r="B57" s="6" t="s">
         <v>88</v>
       </c>
       <c r="C57" s="6" t="s">
-        <v>246</v>
+        <v>196</v>
       </c>
       <c r="D57" s="6" t="s">
         <v>91</v>
       </c>
       <c r="E57" s="6">
-        <v>92161</v>
+        <v>8193</v>
       </c>
       <c r="F57" s="6" t="s">
-        <v>247</v>
+        <v>280</v>
       </c>
       <c r="G57" s="6" t="s">
-        <v>251</v>
+        <v>199</v>
       </c>
       <c r="H57" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I57" s="6" t="s">
-        <v>223</v>
+        <v>180</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A58" s="6" t="s">
-        <v>248</v>
+        <v>197</v>
       </c>
       <c r="B58" s="6" t="s">
         <v>88</v>
       </c>
       <c r="C58" s="6" t="s">
-        <v>249</v>
+        <v>198</v>
       </c>
       <c r="D58" s="6" t="s">
         <v>91</v>
       </c>
       <c r="E58" s="6">
-        <v>92161</v>
+        <v>6145</v>
       </c>
       <c r="F58" s="6" t="s">
-        <v>250</v>
+        <v>281</v>
       </c>
       <c r="G58" s="6" t="s">
-        <v>252</v>
+        <v>200</v>
       </c>
       <c r="H58" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="I58" s="6" t="s">
-        <v>223</v>
+        <v>180</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.2">
@@ -21766,70 +21768,70 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>253</v>
+        <v>201</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>254</v>
+        <v>202</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>255</v>
+        <v>203</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>256</v>
+        <v>204</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="9" t="s">
-        <v>143</v>
+        <v>126</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>257</v>
+        <v>205</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>258</v>
+        <v>206</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>259</v>
+        <v>207</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>256</v>
+        <v>204</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="9" t="s">
-        <v>162</v>
+        <v>139</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>260</v>
+        <v>208</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>261</v>
+        <v>209</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>262</v>
+        <v>210</v>
       </c>
       <c r="E9" s="9" t="s">
-        <v>256</v>
+        <v>204</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="9" t="s">
-        <v>223</v>
+        <v>180</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>263</v>
+        <v>211</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>264</v>
+        <v>212</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>265</v>
+        <v>213</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>266</v>
+        <v>214</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -28981,54 +28983,54 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="s">
-        <v>256</v>
+        <v>204</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>267</v>
+        <v>215</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>268</v>
+        <v>216</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>269</v>
+        <v>217</v>
       </c>
       <c r="E7" s="17" t="s">
-        <v>270</v>
+        <v>218</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>271</v>
+        <v>219</v>
       </c>
       <c r="G7" s="12" t="s">
-        <v>272</v>
+        <v>220</v>
       </c>
       <c r="H7" s="12" t="s">
-        <v>273</v>
+        <v>221</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="12" t="s">
-        <v>266</v>
+        <v>214</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>274</v>
+        <v>222</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>275</v>
+        <v>223</v>
       </c>
       <c r="D8" s="12" t="s">
-        <v>276</v>
+        <v>224</v>
       </c>
       <c r="E8" s="17" t="s">
-        <v>277</v>
+        <v>225</v>
       </c>
       <c r="F8" s="12" t="s">
-        <v>271</v>
+        <v>219</v>
       </c>
       <c r="G8" s="12" t="s">
-        <v>278</v>
+        <v>226</v>
       </c>
       <c r="H8" s="12" t="s">
-        <v>279</v>
+        <v>227</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
@@ -39102,13 +39104,13 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="15" t="s">
-        <v>271</v>
+        <v>219</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>280</v>
+        <v>228</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>281</v>
+        <v>229</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>